<commit_message>
827. Making A Large Island
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Q No.</t>
   </si>
@@ -43,18 +43,34 @@
   <si>
     <t>Date solved</t>
   </si>
+  <si>
+    <t>Arrays (Basics)</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +81,20 @@
     <font>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -214,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +260,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,137 +582,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -684,6 +720,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1219,13 +1267,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A24" sqref="$A24:$XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.890625" customWidth="1"/>
     <col min="2" max="2" width="38.3984375" customWidth="1"/>
@@ -1251,6 +1299,51 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="2:2">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45688</v>
+      </c>
+    </row>
+    <row r="6" ht="18" spans="1:5">
+      <c r="A6">
+        <v>121</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6">
+        <v>45688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1752. Check if Array Is Sorted and Rotated
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Q No.</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Special Array I</t>
+  </si>
+  <si>
+    <t>Arrays,Two pointers</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t>Arrays,Anagram,Hash Table</t>
+  </si>
+  <si>
+    <t>Check if Array Is Sorted and Rotated</t>
+  </si>
+  <si>
+    <t>Arrays,Cycle,Concatenation</t>
   </si>
 </sst>
 </file>
@@ -1267,18 +1285,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.890625" customWidth="1"/>
     <col min="2" max="2" width="38.3984375" customWidth="1"/>
     <col min="3" max="3" width="14.328125" customWidth="1"/>
-    <col min="4" max="4" width="14.5859375" customWidth="1"/>
+    <col min="4" max="4" width="22.78125" customWidth="1"/>
     <col min="5" max="5" width="13.40625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1344,6 +1362,57 @@
         <v>45688</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>3151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>242</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="6">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1752</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6">
+        <v>45690</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
238. Product of Array Except Self
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Q No.</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>Arrays,Cycle,Concatenation</t>
+  </si>
+  <si>
+    <t>Longest Strictly Increasing or Strictly Decreasing Subarray</t>
+  </si>
+  <si>
+    <t>Arrays(Advance)</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Arrays,Prefix and Postfix</t>
   </si>
 </sst>
 </file>
@@ -1285,16 +1300,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.890625" customWidth="1"/>
-    <col min="2" max="2" width="38.3984375" customWidth="1"/>
+    <col min="2" max="2" width="45.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.328125" customWidth="1"/>
     <col min="4" max="4" width="22.78125" customWidth="1"/>
     <col min="5" max="5" width="13.40625" customWidth="1"/>
@@ -1413,6 +1428,45 @@
         <v>45690</v>
       </c>
     </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>3105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6">
+        <v>45691</v>
+      </c>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="2:2">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>238</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6">
+        <v>45691</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1800. Maximum Ascending Subarray Sum
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Q No.</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Longest Strictly Increasing or Strictly Decreasing Subarray</t>
+  </si>
+  <si>
+    <t>Maximum Ascending Subarray Sum</t>
   </si>
   <si>
     <t>Arrays(Advance)</t>
@@ -277,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,12 +464,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,16 +729,16 @@
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1300,10 +1297,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1445,25 +1442,42 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="12" ht="30" customHeight="1" spans="2:2">
-      <c r="B12" s="3" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>1800</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
       </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6">
+        <v>45692</v>
+      </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
+    <row r="13" ht="30" customHeight="1" spans="2:2">
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
         <v>238</v>
       </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="6">
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6">
         <v>45691</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1790. Check if One String Swap Can Make Strings Equal
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Q No.</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Arrays,Prefix and Postfix</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Arrays,Bucket sort,min heap</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +135,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.25"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <color rgb="FFCE9178"/>
+      <color theme="5" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -612,137 +625,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -755,7 +768,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1297,10 +1313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1338,13 +1354,13 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -1353,7 +1369,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>45688</v>
       </c>
     </row>
@@ -1361,7 +1377,7 @@
       <c r="A6">
         <v>121</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
@@ -1370,7 +1386,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>45688</v>
       </c>
     </row>
@@ -1378,7 +1394,7 @@
       <c r="A7">
         <v>3151</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1387,7 +1403,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>45689</v>
       </c>
     </row>
@@ -1395,7 +1411,7 @@
       <c r="A8">
         <v>242</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -1404,7 +1420,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>45689</v>
       </c>
     </row>
@@ -1412,7 +1428,7 @@
       <c r="A9">
         <v>1752</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
@@ -1421,7 +1437,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>45690</v>
       </c>
     </row>
@@ -1429,7 +1445,7 @@
       <c r="A10">
         <v>3105</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
@@ -1438,7 +1454,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>45691</v>
       </c>
     </row>
@@ -1446,7 +1462,7 @@
       <c r="A11">
         <v>1800</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
@@ -1455,7 +1471,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <v>45692</v>
       </c>
     </row>
@@ -1468,7 +1484,7 @@
       <c r="A15">
         <v>238</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
@@ -1477,8 +1493,25 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <v>45691</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>347</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="7">
+        <v>45692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3160. Find the Number of Distinct Colors Among the Balls
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Q No.</t>
   </si>
@@ -107,6 +107,12 @@
     <t>Arrays,Bucket sort,min heap</t>
   </si>
   <si>
+    <t>Tuple with Same Product</t>
+  </si>
+  <si>
+    <t>Arrays,hashmap,Counting,Combinations</t>
+  </si>
+  <si>
     <t>Two pointers (Basics)</t>
   </si>
   <si>
@@ -114,6 +120,12 @@
   </si>
   <si>
     <t>String,Two pointers,Comparison</t>
+  </si>
+  <si>
+    <t>Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>Arrays,Two pointers,Binary Search</t>
   </si>
 </sst>
 </file>
@@ -777,7 +789,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -795,9 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1341,10 +1350,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1352,7 +1361,7 @@
     <col min="1" max="1" width="12.890625" customWidth="1"/>
     <col min="2" max="2" width="45.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.328125" customWidth="1"/>
-    <col min="4" max="4" width="27.3359375" customWidth="1"/>
+    <col min="4" max="4" width="42.3203125" customWidth="1"/>
     <col min="5" max="5" width="13.40625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1382,7 +1391,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1397,7 +1406,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>45688</v>
       </c>
     </row>
@@ -1414,7 +1423,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>45688</v>
       </c>
     </row>
@@ -1431,7 +1440,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>45689</v>
       </c>
     </row>
@@ -1448,7 +1457,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>45689</v>
       </c>
     </row>
@@ -1465,7 +1474,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>45690</v>
       </c>
     </row>
@@ -1482,7 +1491,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>45691</v>
       </c>
     </row>
@@ -1499,7 +1508,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>45692</v>
       </c>
     </row>
@@ -1516,7 +1525,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>45693</v>
       </c>
     </row>
@@ -1538,7 +1547,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>45691</v>
       </c>
     </row>
@@ -1555,30 +1564,64 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>45692</v>
       </c>
     </row>
-    <row r="19" ht="25" customHeight="1" spans="2:2">
-      <c r="B19" s="6" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>1726</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="8">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="20" ht="25" customHeight="1" spans="2:2">
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
         <v>125</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="9">
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="8">
         <v>45693</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>167</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="8">
+        <v>45694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11. Container With Most Water
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="13660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Q No.</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Arrays,Two pointers,Binary Search</t>
+  </si>
+  <si>
+    <t>Two pointers (Advance)</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Arrays,Two Pointer,Comparison</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1359,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1624,6 +1633,28 @@
         <v>45694</v>
       </c>
     </row>
+    <row r="25" ht="39" customHeight="1" spans="2:2">
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="8">
+        <v>45695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2364. Count Number of Bad Pairs
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13660"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Q No.</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Arrays,hashmap,Counting,Combinations</t>
+  </si>
+  <si>
+    <t>Count Number of Bad Pairs</t>
   </si>
   <si>
     <t>Two pointers (Basics)</t>
@@ -1359,10 +1362,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1594,64 +1597,81 @@
         <v>45694</v>
       </c>
     </row>
-    <row r="20" ht="25" customHeight="1" spans="2:2">
-      <c r="B20" s="3" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>2364</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>125</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="8">
+        <v>45697</v>
+      </c>
+    </row>
+    <row r="21" ht="25" customHeight="1" spans="2:2">
+      <c r="B21" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="8">
-        <v>45693</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
+        <v>125</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="8">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
         <v>167</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="8">
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="8">
         <v>45694</v>
       </c>
     </row>
-    <row r="25" ht="39" customHeight="1" spans="2:2">
-      <c r="B25" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
+    <row r="26" ht="39" customHeight="1" spans="2:2">
+      <c r="B26" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
         <v>11</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="8">
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="8">
         <v>45695</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2342. Max Sum of a Pair With Equal Sum of Digits
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Q No.</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Arrays,Two Pointer,Comparison</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t>Arrays,Two Pointers ,Sorting</t>
   </si>
 </sst>
 </file>
@@ -1362,10 +1368,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1675,6 +1681,23 @@
         <v>45695</v>
       </c>
     </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="8">
+        <v>45699</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
3066. Minimum Operations to Exceed Threshold Value II
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Q No.</t>
   </si>
@@ -116,6 +116,9 @@
     <t>Count Number of Bad Pairs</t>
   </si>
   <si>
+    <t>Max Sum of a Pair With Equal Sum of Digits</t>
+  </si>
+  <si>
     <t>Two pointers (Basics)</t>
   </si>
   <si>
@@ -144,6 +147,15 @@
   </si>
   <si>
     <t>Arrays,Two Pointers ,Sorting</t>
+  </si>
+  <si>
+    <t>Sliding Window (Basics)</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>String,Sliding Window,Two pointers</t>
   </si>
 </sst>
 </file>
@@ -157,7 +169,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,13 +201,6 @@
     <font>
       <sz val="12"/>
       <color theme="5" tint="-0.25"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -677,137 +682,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -825,9 +830,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1368,10 +1370,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1409,7 +1411,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1424,7 +1426,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>45688</v>
       </c>
     </row>
@@ -1441,7 +1443,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>45688</v>
       </c>
     </row>
@@ -1458,7 +1460,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>45689</v>
       </c>
     </row>
@@ -1475,7 +1477,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>45689</v>
       </c>
     </row>
@@ -1492,7 +1494,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>45690</v>
       </c>
     </row>
@@ -1509,7 +1511,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>45691</v>
       </c>
     </row>
@@ -1526,7 +1528,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>45692</v>
       </c>
     </row>
@@ -1543,7 +1545,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>45693</v>
       </c>
     </row>
@@ -1565,7 +1567,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>45691</v>
       </c>
     </row>
@@ -1582,7 +1584,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>45692</v>
       </c>
     </row>
@@ -1599,7 +1601,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>45694</v>
       </c>
     </row>
@@ -1607,7 +1609,7 @@
       <c r="A19">
         <v>2364</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
@@ -1616,86 +1618,125 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>45697</v>
       </c>
     </row>
-    <row r="21" ht="25" customHeight="1" spans="2:2">
-      <c r="B21" s="3" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>2342</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>125</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="7">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="22" ht="25" customHeight="1" spans="2:2">
+      <c r="B22" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="8">
-        <v>45693</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
+        <v>125</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="7">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>167</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="8">
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="7">
         <v>45694</v>
       </c>
     </row>
-    <row r="26" ht="39" customHeight="1" spans="2:2">
-      <c r="B26" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>11</v>
-      </c>
-      <c r="B28" s="6" t="s">
+    <row r="27" ht="39" customHeight="1" spans="2:2">
+      <c r="B27" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="8">
-        <v>45695</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>15</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
       </c>
       <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="7">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="8">
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="7">
         <v>45699</v>
+      </c>
+    </row>
+    <row r="32" ht="32" customHeight="1" spans="2:2">
+      <c r="B32" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="7">
+        <v>45700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
567. Permutation in String
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Q No.</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>String,Sliding Window,Two pointers</t>
+  </si>
+  <si>
+    <t>Permutation in String</t>
+  </si>
+  <si>
+    <t>String,Sliding Window,Counter</t>
   </si>
 </sst>
 </file>
@@ -1370,10 +1376,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1739,6 +1745,23 @@
         <v>45700</v>
       </c>
     </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>567</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="7">
+        <v>45701</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix : exel updation
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Q No.</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>String,Sliding Window,Counter</t>
+  </si>
+  <si>
+    <t>Heap (Basics)</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Exceed Threshold Value II</t>
+  </si>
+  <si>
+    <t>Array,Min Heap</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +216,13 @@
     <font>
       <sz val="12"/>
       <color theme="5" tint="-0.25"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -356,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +394,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,55 +710,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -751,74 +770,77 @@
     <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -836,6 +858,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1376,10 +1401,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1417,7 +1442,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1432,7 +1457,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>45688</v>
       </c>
     </row>
@@ -1449,7 +1474,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>45688</v>
       </c>
     </row>
@@ -1466,7 +1491,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>45689</v>
       </c>
     </row>
@@ -1483,7 +1508,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="8">
         <v>45689</v>
       </c>
     </row>
@@ -1500,7 +1525,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <v>45690</v>
       </c>
     </row>
@@ -1517,7 +1542,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
         <v>45691</v>
       </c>
     </row>
@@ -1534,7 +1559,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <v>45692</v>
       </c>
     </row>
@@ -1551,7 +1576,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="8">
         <v>45693</v>
       </c>
     </row>
@@ -1573,7 +1598,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <v>45691</v>
       </c>
     </row>
@@ -1590,7 +1615,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <v>45692</v>
       </c>
     </row>
@@ -1607,7 +1632,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <v>45694</v>
       </c>
     </row>
@@ -1624,7 +1649,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <v>45697</v>
       </c>
     </row>
@@ -1641,7 +1666,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <v>45700</v>
       </c>
     </row>
@@ -1663,7 +1688,7 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="8">
         <v>45693</v>
       </c>
     </row>
@@ -1680,11 +1705,11 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="8">
         <v>45694</v>
       </c>
     </row>
-    <row r="27" ht="39" customHeight="1" spans="2:2">
+    <row r="27" ht="31" customHeight="1" spans="2:2">
       <c r="B27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1702,7 +1727,7 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="8">
         <v>45695</v>
       </c>
     </row>
@@ -1719,7 +1744,7 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="8">
         <v>45699</v>
       </c>
     </row>
@@ -1741,7 +1766,7 @@
       <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="8">
         <v>45700</v>
       </c>
     </row>
@@ -1758,7 +1783,29 @@
       <c r="D35" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="8">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="37" ht="31" customHeight="1" spans="2:2">
+      <c r="B37" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>3066</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="8">
         <v>45701</v>
       </c>
     </row>

</xml_diff>

<commit_message>
424. Longest Repeating Character Replacement
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Q No.</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>String,Sliding Window,Counter</t>
+  </si>
+  <si>
+    <t>Sliding Window (Advance)</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>String,sliding window,hashmap</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -840,7 +849,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -857,6 +866,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1401,10 +1413,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1442,7 +1454,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1457,7 +1469,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <v>45688</v>
       </c>
     </row>
@@ -1474,7 +1486,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>45688</v>
       </c>
     </row>
@@ -1491,7 +1503,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>45689</v>
       </c>
     </row>
@@ -1508,7 +1520,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>45689</v>
       </c>
     </row>
@@ -1525,7 +1537,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>45690</v>
       </c>
     </row>
@@ -1542,7 +1554,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>45691</v>
       </c>
     </row>
@@ -1559,7 +1571,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="9">
         <v>45692</v>
       </c>
     </row>
@@ -1576,7 +1588,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="9">
         <v>45693</v>
       </c>
     </row>
@@ -1598,7 +1610,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="9">
         <v>45691</v>
       </c>
     </row>
@@ -1615,7 +1627,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="9">
         <v>45692</v>
       </c>
     </row>
@@ -1632,7 +1644,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="9">
         <v>45694</v>
       </c>
     </row>
@@ -1649,7 +1661,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="9">
         <v>45697</v>
       </c>
     </row>
@@ -1666,7 +1678,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="9">
         <v>45700</v>
       </c>
     </row>
@@ -1688,7 +1700,7 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="9">
         <v>45693</v>
       </c>
     </row>
@@ -1705,7 +1717,7 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="9">
         <v>45694</v>
       </c>
     </row>
@@ -1727,7 +1739,7 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="9">
         <v>45695</v>
       </c>
     </row>
@@ -1744,7 +1756,7 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="9">
         <v>45699</v>
       </c>
     </row>
@@ -1766,7 +1778,7 @@
       <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="9">
         <v>45700</v>
       </c>
     </row>
@@ -1783,20 +1795,24 @@
       <c r="D35" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="9">
         <v>45701</v>
       </c>
     </row>
-    <row r="37" ht="31" customHeight="1" spans="2:2">
-      <c r="B37" s="6" t="s">
+    <row r="36" spans="2:5">
+      <c r="B36" s="4"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" ht="39" customHeight="1" spans="2:2">
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" ht="17" spans="1:5">
       <c r="A39">
-        <v>3066</v>
-      </c>
-      <c r="B39" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C39" t="s">
@@ -1805,7 +1821,29 @@
       <c r="D39" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="9">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="42" ht="31" customHeight="1" spans="2:2">
+      <c r="B42" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>3066</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="9">
         <v>45701</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1780. Check if Number is a Sum of Powers of Three
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Q No.</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>Array,Min Heap</t>
+  </si>
+  <si>
+    <t>Stack (Basics)</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Arrays , Stack</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1422,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1847,6 +1856,28 @@
         <v>45701</v>
       </c>
     </row>
+    <row r="46" ht="38" customHeight="1" spans="2:2">
+      <c r="B46" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="9">
+        <v>45719</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
226. Invert Binary Tree(recursion)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Q No.</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Monotonic Stack</t>
+  </si>
+  <si>
+    <t>Binary Tree (basic)</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Tree,recurson</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1446,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1932,6 +1941,28 @@
         <v>45732</v>
       </c>
     </row>
+    <row r="55" ht="35" customHeight="1" spans="2:2">
+      <c r="B55" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>226</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>61</v>
+      </c>
+      <c r="E57" s="9">
+        <v>45733</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
84. Largest Rectangle in Histogram (stack -advance)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Q No.</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Monotonic Stack</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>Hard</t>
   </si>
   <si>
     <t>Binary Tree (basic)</t>
@@ -1446,10 +1452,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D55" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1941,25 +1947,42 @@
         <v>45732</v>
       </c>
     </row>
-    <row r="55" ht="35" customHeight="1" spans="2:2">
-      <c r="B55" s="7" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57">
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" s="9">
+        <v>45745</v>
+      </c>
+    </row>
+    <row r="56" ht="35" customHeight="1" spans="2:2">
+      <c r="B56" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
         <v>226</v>
       </c>
-      <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
         <v>7</v>
       </c>
-      <c r="D57" t="s">
-        <v>61</v>
-      </c>
-      <c r="E57" s="9">
+      <c r="D58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="9">
         <v>45733</v>
       </c>
     </row>

</xml_diff>

<commit_message>
206. Reverse Linked List
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Q No.</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>Hard</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Linked List ,Three pointers(iterative) , recursive</t>
   </si>
   <si>
     <t>Binary Tree (basic)</t>
@@ -238,8 +247,16 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="26">
-    <font>
+  <fonts count="29">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -284,6 +301,21 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -771,168 +803,183 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1468,10 +1515,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1484,38 +1531,38 @@
   </cols>
   <sheetData>
     <row r="1" ht="39" customHeight="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:2">
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="2:2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="9"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -1524,7 +1571,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="13">
         <v>45688</v>
       </c>
     </row>
@@ -1532,7 +1579,7 @@
       <c r="A6">
         <v>121</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
@@ -1541,7 +1588,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="14">
         <v>45688</v>
       </c>
     </row>
@@ -1549,7 +1596,7 @@
       <c r="A7">
         <v>3151</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1558,7 +1605,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="14">
         <v>45689</v>
       </c>
     </row>
@@ -1566,7 +1613,7 @@
       <c r="A8">
         <v>242</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -1575,7 +1622,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="14">
         <v>45689</v>
       </c>
     </row>
@@ -1583,7 +1630,7 @@
       <c r="A9">
         <v>1752</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
@@ -1592,7 +1639,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="14">
         <v>45690</v>
       </c>
     </row>
@@ -1600,7 +1647,7 @@
       <c r="A10">
         <v>3105</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
@@ -1609,7 +1656,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="14">
         <v>45691</v>
       </c>
     </row>
@@ -1617,7 +1664,7 @@
       <c r="A11">
         <v>1800</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
@@ -1626,7 +1673,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="14">
         <v>45692</v>
       </c>
     </row>
@@ -1634,7 +1681,7 @@
       <c r="A12">
         <v>1790</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
@@ -1643,12 +1690,12 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="14">
         <v>45693</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1" spans="2:2">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1656,7 +1703,7 @@
       <c r="A16">
         <v>238</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
@@ -1665,7 +1712,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="14">
         <v>45691</v>
       </c>
     </row>
@@ -1673,7 +1720,7 @@
       <c r="A17">
         <v>347</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C17" t="s">
@@ -1682,7 +1729,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="14">
         <v>45692</v>
       </c>
     </row>
@@ -1690,7 +1737,7 @@
       <c r="A18">
         <v>1726</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
@@ -1699,7 +1746,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="14">
         <v>45694</v>
       </c>
     </row>
@@ -1707,7 +1754,7 @@
       <c r="A19">
         <v>2364</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
@@ -1716,7 +1763,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="14">
         <v>45697</v>
       </c>
     </row>
@@ -1724,7 +1771,7 @@
       <c r="A20">
         <v>2342</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C20" t="s">
@@ -1733,12 +1780,12 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="14">
         <v>45700</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1" spans="2:2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1746,7 +1793,7 @@
       <c r="A24">
         <v>125</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C24" t="s">
@@ -1755,7 +1802,7 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="14">
         <v>45693</v>
       </c>
     </row>
@@ -1763,7 +1810,7 @@
       <c r="A25">
         <v>167</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C25" t="s">
@@ -1772,12 +1819,12 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="14">
         <v>45694</v>
       </c>
     </row>
     <row r="27" ht="31" customHeight="1" spans="2:2">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1785,7 +1832,7 @@
       <c r="A29">
         <v>11</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C29" t="s">
@@ -1794,7 +1841,7 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="14">
         <v>45695</v>
       </c>
     </row>
@@ -1802,7 +1849,7 @@
       <c r="A30">
         <v>15</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C30" t="s">
@@ -1811,7 +1858,7 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="14">
         <v>45699</v>
       </c>
     </row>
@@ -1819,7 +1866,7 @@
       <c r="A31">
         <v>763</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C31" t="s">
@@ -1828,12 +1875,12 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="14">
         <v>45746</v>
       </c>
     </row>
     <row r="33" ht="32" customHeight="1" spans="2:2">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1841,7 +1888,7 @@
       <c r="A35">
         <v>3</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C35" t="s">
@@ -1850,7 +1897,7 @@
       <c r="D35" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="14">
         <v>45700</v>
       </c>
     </row>
@@ -1858,7 +1905,7 @@
       <c r="A36">
         <v>567</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C36" t="s">
@@ -1867,16 +1914,16 @@
       <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="14">
         <v>45701</v>
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="4"/>
-      <c r="E37" s="10"/>
+      <c r="B37" s="5"/>
+      <c r="E37" s="14"/>
     </row>
     <row r="38" ht="39" customHeight="1" spans="2:2">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1884,7 +1931,7 @@
       <c r="A40">
         <v>424</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
@@ -1893,12 +1940,12 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="14">
         <v>45716</v>
       </c>
     </row>
     <row r="43" ht="31" customHeight="1" spans="2:2">
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1906,7 +1953,7 @@
       <c r="A45">
         <v>3066</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C45" t="s">
@@ -1915,12 +1962,12 @@
       <c r="D45" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="14">
         <v>45701</v>
       </c>
     </row>
     <row r="47" ht="38" customHeight="1" spans="2:2">
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="9" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1928,7 +1975,7 @@
       <c r="A49">
         <v>20</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C49" t="s">
@@ -1937,7 +1984,7 @@
       <c r="D49" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="14">
         <v>45719</v>
       </c>
     </row>
@@ -1945,7 +1992,7 @@
       <c r="A50">
         <v>155</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C50" t="s">
@@ -1954,12 +2001,12 @@
       <c r="D50" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="14">
         <v>45731</v>
       </c>
     </row>
     <row r="52" ht="40" customHeight="1" spans="2:2">
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1967,7 +2014,7 @@
       <c r="A54">
         <v>739</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C54" t="s">
@@ -1976,37 +2023,39 @@
       <c r="D54" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54" s="14">
         <v>45732</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55">
+    <row r="55" s="1" customFormat="1" spans="1:5">
+      <c r="A55" s="1">
         <v>84</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="15">
         <v>45745</v>
       </c>
     </row>
-    <row r="57" ht="35" customHeight="1" spans="2:2">
-      <c r="B57" s="8" t="s">
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="58" customFormat="1"/>
+    <row r="59" customFormat="1" ht="18" spans="1:5">
       <c r="A59">
-        <v>226</v>
-      </c>
-      <c r="B59" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C59" t="s">
@@ -2015,7 +2064,29 @@
       <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="14">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="61" ht="35" customHeight="1" spans="2:2">
+      <c r="B61" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>226</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="14">
         <v>45733</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Q2. Add Two Numbers.py & Q21. Merge Two Sorted Lists
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>Q No.</t>
   </si>
@@ -218,13 +218,25 @@
     <t>Hard</t>
   </si>
   <si>
-    <t>Linked List</t>
+    <t>Linked List (Basics)</t>
   </si>
   <si>
     <t>Reverse Linked List</t>
   </si>
   <si>
     <t>Linked List ,Three pointers(iterative) , recursive</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked List </t>
+  </si>
+  <si>
+    <t>Linked List (Advanced)</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
   </si>
   <si>
     <t>Binary Tree (basic)</t>
@@ -933,7 +945,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -965,9 +977,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1515,10 +1524,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1556,7 +1565,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1571,7 +1580,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>45688</v>
       </c>
     </row>
@@ -1588,7 +1597,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>45688</v>
       </c>
     </row>
@@ -1605,7 +1614,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>45689</v>
       </c>
     </row>
@@ -1622,7 +1631,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>45689</v>
       </c>
     </row>
@@ -1639,7 +1648,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>45690</v>
       </c>
     </row>
@@ -1656,7 +1665,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>45691</v>
       </c>
     </row>
@@ -1673,7 +1682,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>45692</v>
       </c>
     </row>
@@ -1690,7 +1699,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>45693</v>
       </c>
     </row>
@@ -1712,7 +1721,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>45691</v>
       </c>
     </row>
@@ -1729,7 +1738,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>45692</v>
       </c>
     </row>
@@ -1746,7 +1755,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>45694</v>
       </c>
     </row>
@@ -1763,7 +1772,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>45697</v>
       </c>
     </row>
@@ -1780,7 +1789,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>45700</v>
       </c>
     </row>
@@ -1802,7 +1811,7 @@
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <v>45693</v>
       </c>
     </row>
@@ -1819,7 +1828,7 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <v>45694</v>
       </c>
     </row>
@@ -1841,7 +1850,7 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="13">
         <v>45695</v>
       </c>
     </row>
@@ -1858,7 +1867,7 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <v>45699</v>
       </c>
     </row>
@@ -1875,7 +1884,7 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <v>45746</v>
       </c>
     </row>
@@ -1897,7 +1906,7 @@
       <c r="D35" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="13">
         <v>45700</v>
       </c>
     </row>
@@ -1914,13 +1923,13 @@
       <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="13">
         <v>45701</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="5"/>
-      <c r="E37" s="14"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" ht="39" customHeight="1" spans="2:2">
       <c r="B38" s="4" t="s">
@@ -1940,7 +1949,7 @@
       <c r="D40" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="13">
         <v>45716</v>
       </c>
     </row>
@@ -1962,7 +1971,7 @@
       <c r="D45" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="13">
         <v>45701</v>
       </c>
     </row>
@@ -1984,7 +1993,7 @@
       <c r="D49" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="13">
         <v>45719</v>
       </c>
     </row>
@@ -2001,7 +2010,7 @@
       <c r="D50" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="13">
         <v>45731</v>
       </c>
     </row>
@@ -2023,7 +2032,7 @@
       <c r="D54" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="13">
         <v>45732</v>
       </c>
     </row>
@@ -2034,28 +2043,26 @@
       <c r="B55" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="14">
         <v>45745</v>
       </c>
     </row>
-    <row r="56" customFormat="1"/>
     <row r="57" customFormat="1" ht="31" customHeight="1" spans="2:2">
       <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" customFormat="1"/>
     <row r="59" customFormat="1" ht="18" spans="1:5">
       <c r="A59">
         <v>206</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C59" t="s">
@@ -2064,29 +2071,75 @@
       <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="14">
+      <c r="E59" s="13">
         <v>45746</v>
       </c>
     </row>
-    <row r="61" ht="35" customHeight="1" spans="2:2">
-      <c r="B61" s="9" t="s">
+    <row r="60" customFormat="1" spans="1:5">
+      <c r="A60">
+        <v>21</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63">
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="13">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" spans="5:5">
+      <c r="E61" s="13"/>
+    </row>
+    <row r="62" customFormat="1" spans="2:5">
+      <c r="B62" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" customFormat="1" spans="5:5">
+      <c r="E63" s="13"/>
+    </row>
+    <row r="64" customFormat="1" spans="1:5">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" s="13">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="66" ht="35" customHeight="1" spans="2:2">
+      <c r="B66" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
         <v>226</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B68" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" t="s">
         <v>7</v>
       </c>
-      <c r="D63" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="14">
+      <c r="D68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" s="13">
         <v>45733</v>
       </c>
     </row>

</xml_diff>

<commit_message>
33. Search in Rotated Sorted Array
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>Q No.</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Binary Search , recursion</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Binary Search ,left and right portion</t>
   </si>
 </sst>
 </file>
@@ -1539,10 +1545,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2197,6 +2203,23 @@
         <v>45757</v>
       </c>
     </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" t="s">
+        <v>79</v>
+      </c>
+      <c r="E74" s="13">
+        <v>45759</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2799. Count Complete Subarrays in an Array
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>Q No.</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>String,sliding window,hashmap</t>
+  </si>
+  <si>
+    <t>Count Complete Subarrays in an Array</t>
+  </si>
+  <si>
+    <t>Arrays ,Sliding Window</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -1545,10 +1551,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1974,9 +1980,26 @@
         <v>45716</v>
       </c>
     </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>2799</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="13">
+        <v>45771</v>
+      </c>
+    </row>
     <row r="43" ht="31" customHeight="1" spans="2:2">
       <c r="B43" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1984,13 +2007,13 @@
         <v>3066</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E45" s="13">
         <v>45701</v>
@@ -1998,7 +2021,7 @@
     </row>
     <row r="47" ht="38" customHeight="1" spans="2:2">
       <c r="B47" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2006,13 +2029,13 @@
         <v>20</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E49" s="13">
         <v>45719</v>
@@ -2023,13 +2046,13 @@
         <v>155</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
         <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E50" s="13">
         <v>45731</v>
@@ -2037,7 +2060,7 @@
     </row>
     <row r="52" ht="40" customHeight="1" spans="2:2">
       <c r="B52" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2045,13 +2068,13 @@
         <v>739</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
         <v>22</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E54" s="13">
         <v>45732</v>
@@ -2062,45 +2085,29 @@
         <v>84</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E55" s="14">
         <v>45745</v>
       </c>
     </row>
-    <row r="57" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B57" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" customFormat="1" ht="18" spans="1:5">
-      <c r="A59">
+    <row r="56" customFormat="1"/>
+    <row r="58" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B58" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" customFormat="1" ht="18" spans="1:5">
+      <c r="A60">
         <v>206</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="13">
-        <v>45746</v>
-      </c>
-    </row>
-    <row r="60" customFormat="1" spans="1:5">
-      <c r="A60">
-        <v>21</v>
-      </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C60" t="s">
@@ -2110,113 +2117,130 @@
         <v>67</v>
       </c>
       <c r="E60" s="13">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" spans="1:5">
+      <c r="A61">
+        <v>21</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="13">
         <v>45747</v>
       </c>
     </row>
-    <row r="61" customFormat="1" spans="5:5">
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" customFormat="1" spans="2:5">
-      <c r="B62" s="4" t="s">
-        <v>68</v>
-      </c>
+    <row r="62" customFormat="1" spans="5:5">
       <c r="E62" s="13"/>
     </row>
-    <row r="63" customFormat="1" spans="5:5">
+    <row r="63" customFormat="1" spans="2:5">
+      <c r="B63" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="E63" s="13"/>
     </row>
-    <row r="64" customFormat="1" spans="1:5">
-      <c r="A64">
-        <v>2</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" t="s">
-        <v>22</v>
-      </c>
-      <c r="D64" t="s">
-        <v>67</v>
-      </c>
-      <c r="E64" s="13">
-        <v>45747</v>
-      </c>
+    <row r="64" customFormat="1" spans="5:5">
+      <c r="E64" s="13"/>
     </row>
     <row r="65" customFormat="1" spans="1:5">
       <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="13">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" spans="1:5">
+      <c r="A66">
         <v>141</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B66" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" t="s">
         <v>7</v>
       </c>
-      <c r="D65" t="s">
-        <v>71</v>
-      </c>
-      <c r="E65" s="13">
+      <c r="D66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" s="13">
         <v>45748</v>
       </c>
     </row>
-    <row r="67" ht="35" customHeight="1" spans="2:2">
-      <c r="B67" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69">
+    <row r="68" ht="35" customHeight="1" spans="2:2">
+      <c r="B68" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
         <v>226</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B70" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" t="s">
         <v>7</v>
       </c>
-      <c r="D69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E69" s="13">
+      <c r="D70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" s="13">
         <v>45733</v>
       </c>
     </row>
-    <row r="71" ht="39" customHeight="1" spans="2:2">
-      <c r="B71" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73">
-        <v>704</v>
-      </c>
-      <c r="B73" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" t="s">
+    <row r="72" ht="39" customHeight="1" spans="2:2">
+      <c r="B72" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="E73" s="13">
-        <v>45757</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B74" t="s">
         <v>78</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
         <v>79</v>
       </c>
       <c r="E74" s="13">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" t="s">
+        <v>81</v>
+      </c>
+      <c r="E75" s="13">
         <v>45759</v>
       </c>
     </row>

</xml_diff>

<commit_message>
34. Find First and Last Position of Element in Sorted Array
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
   <si>
     <t>Q No.</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>Binary Search ,left and right portion</t>
+  </si>
+  <si>
+    <t>Binary Search (Advance)</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t>Binary Search , leftBiased</t>
   </si>
 </sst>
 </file>
@@ -286,7 +295,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +364,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFCE9178"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -842,137 +858,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1017,6 +1033,9 @@
     </xf>
     <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1551,16 +1570,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.890625" customWidth="1"/>
-    <col min="2" max="2" width="45.1796875" customWidth="1"/>
+    <col min="2" max="2" width="61.453125" customWidth="1"/>
     <col min="3" max="3" width="14.328125" customWidth="1"/>
     <col min="4" max="4" width="42.3203125" customWidth="1"/>
     <col min="5" max="5" width="13.40625" customWidth="1"/>
@@ -2097,7 +2116,6 @@
         <v>45745</v>
       </c>
     </row>
-    <row r="56" customFormat="1"/>
     <row r="58" customFormat="1" ht="31" customHeight="1" spans="2:2">
       <c r="B58" s="4" t="s">
         <v>65</v>
@@ -2214,7 +2232,7 @@
       <c r="A74">
         <v>704</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C74" t="s">
@@ -2231,7 +2249,7 @@
       <c r="A75">
         <v>33</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C75" t="s">
@@ -2242,6 +2260,28 @@
       </c>
       <c r="E75" s="13">
         <v>45759</v>
+      </c>
+    </row>
+    <row r="77" ht="32" customHeight="1" spans="2:2">
+      <c r="B77" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" ht="30" customHeight="1" spans="1:5">
+      <c r="A79">
+        <v>34</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" t="s">
+        <v>84</v>
+      </c>
+      <c r="E79" s="13">
+        <v>45773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs : updated  tracker sheet
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
   <si>
     <t>Q No.</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Binary Search , leftBiased</t>
+  </si>
+  <si>
+    <t>Trees ( Basics )</t>
+  </si>
+  <si>
+    <t>Tree ,Binary tree</t>
   </si>
 </sst>
 </file>
@@ -1570,10 +1576,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2284,6 +2290,28 @@
         <v>45773</v>
       </c>
     </row>
+    <row r="81" ht="29" customHeight="1" spans="2:2">
+      <c r="B81" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>226</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" s="13">
+        <v>45774</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2962. Count Subarrays Where Max Element Appears at Least K Times (Sliding window)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>Q No.</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Arrays ,Sliding Window</t>
+  </si>
+  <si>
+    <t>Count Subarrays Where Max Element Appears at Least K Times</t>
+  </si>
+  <si>
+    <t>Arrays ,Sliding Window ,Count</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -1576,10 +1582,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2022,133 +2028,133 @@
         <v>45771</v>
       </c>
     </row>
-    <row r="43" ht="31" customHeight="1" spans="2:2">
-      <c r="B43" s="9" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>2962</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45">
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="13">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="44" ht="31" customHeight="1" spans="2:2">
+      <c r="B44" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
         <v>3066</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="D45" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="13">
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="13">
         <v>45701</v>
       </c>
     </row>
-    <row r="47" ht="38" customHeight="1" spans="2:2">
-      <c r="B47" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49">
-        <v>20</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" t="s">
+    <row r="48" ht="38" customHeight="1" spans="2:2">
+      <c r="B48" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="E49" s="13">
-        <v>45719</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
         <v>59</v>
       </c>
       <c r="E50" s="13">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>155</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="13">
         <v>45731</v>
       </c>
     </row>
-    <row r="52" ht="40" customHeight="1" spans="2:2">
-      <c r="B52" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54">
+    <row r="53" ht="40" customHeight="1" spans="2:2">
+      <c r="B53" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
         <v>739</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B55" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" t="s">
         <v>22</v>
       </c>
-      <c r="D54" t="s">
-        <v>62</v>
-      </c>
-      <c r="E54" s="13">
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="13">
         <v>45732</v>
       </c>
     </row>
-    <row r="55" s="1" customFormat="1" spans="1:5">
-      <c r="A55" s="1">
+    <row r="56" s="1" customFormat="1" spans="1:5">
+      <c r="A56" s="1">
         <v>84</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B56" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" s="14">
+      <c r="E56" s="14">
         <v>45745</v>
       </c>
     </row>
-    <row r="58" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B58" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" customFormat="1" ht="18" spans="1:5">
-      <c r="A60">
+    <row r="59" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B59" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" ht="18" spans="1:5">
+      <c r="A61">
         <v>206</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" s="13">
-        <v>45746</v>
-      </c>
-    </row>
-    <row r="61" customFormat="1" spans="1:5">
-      <c r="A61">
-        <v>21</v>
-      </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C61" t="s">
@@ -2158,157 +2164,174 @@
         <v>69</v>
       </c>
       <c r="E61" s="13">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="62" customFormat="1" spans="1:5">
+      <c r="A62">
+        <v>21</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" s="13">
         <v>45747</v>
       </c>
     </row>
-    <row r="62" customFormat="1" spans="5:5">
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" customFormat="1" spans="2:5">
-      <c r="B63" s="4" t="s">
-        <v>70</v>
-      </c>
+    <row r="63" customFormat="1" spans="5:5">
       <c r="E63" s="13"/>
     </row>
-    <row r="64" customFormat="1" spans="5:5">
+    <row r="64" customFormat="1" spans="2:5">
+      <c r="B64" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="E64" s="13"/>
     </row>
-    <row r="65" customFormat="1" spans="1:5">
-      <c r="A65">
-        <v>2</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" t="s">
-        <v>69</v>
-      </c>
-      <c r="E65" s="13">
-        <v>45747</v>
-      </c>
+    <row r="65" customFormat="1" spans="5:5">
+      <c r="E65" s="13"/>
     </row>
     <row r="66" customFormat="1" spans="1:5">
       <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" s="13">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" spans="1:5">
+      <c r="A67">
         <v>141</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B67" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" t="s">
         <v>7</v>
       </c>
-      <c r="D66" t="s">
-        <v>73</v>
-      </c>
-      <c r="E66" s="13">
+      <c r="D67" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" s="13">
         <v>45748</v>
       </c>
     </row>
-    <row r="68" ht="35" customHeight="1" spans="2:2">
-      <c r="B68" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70">
+    <row r="69" ht="35" customHeight="1" spans="2:2">
+      <c r="B69" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
         <v>226</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B71" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
         <v>7</v>
       </c>
-      <c r="D70" t="s">
-        <v>76</v>
-      </c>
-      <c r="E70" s="13">
+      <c r="D71" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="13">
         <v>45733</v>
       </c>
     </row>
-    <row r="72" ht="39" customHeight="1" spans="2:2">
-      <c r="B72" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74">
-        <v>704</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" t="s">
+    <row r="73" ht="39" customHeight="1" spans="2:2">
+      <c r="B73" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="E74" s="13">
-        <v>45757</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D75" t="s">
         <v>81</v>
       </c>
       <c r="E75" s="13">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>33</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" t="s">
+        <v>83</v>
+      </c>
+      <c r="E76" s="13">
         <v>45759</v>
       </c>
     </row>
-    <row r="77" ht="32" customHeight="1" spans="2:2">
-      <c r="B77" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" ht="30" customHeight="1" spans="1:5">
-      <c r="A79">
+    <row r="78" ht="32" customHeight="1" spans="2:2">
+      <c r="B78" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" ht="30" customHeight="1" spans="1:5">
+      <c r="A80">
         <v>34</v>
       </c>
-      <c r="B79" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B80" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" t="s">
         <v>22</v>
       </c>
-      <c r="D79" t="s">
-        <v>84</v>
-      </c>
-      <c r="E79" s="13">
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" s="13">
         <v>45773</v>
       </c>
     </row>
-    <row r="81" ht="29" customHeight="1" spans="2:2">
-      <c r="B81" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83">
+    <row r="82" ht="29" customHeight="1" spans="2:2">
+      <c r="B82" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
         <v>226</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="B84" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" t="s">
         <v>7</v>
       </c>
-      <c r="D83" t="s">
-        <v>86</v>
-      </c>
-      <c r="E83" s="13">
+      <c r="D84" t="s">
+        <v>88</v>
+      </c>
+      <c r="E84" s="13">
         <v>45774</v>
       </c>
     </row>

</xml_diff>

<commit_message>
104. Maximum Depth of Binary Tree (BFS , DFS)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Q No.</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Tree ,Binary tree</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>BFS ,DFS  recursion</t>
   </si>
 </sst>
 </file>
@@ -1582,10 +1588,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2335,6 +2341,23 @@
         <v>45774</v>
       </c>
     </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>104</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>90</v>
+      </c>
+      <c r="E85" s="13">
+        <v>45782</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
100. Same Tree (Trees-easy)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
   <si>
     <t>Q No.</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>BFS ,DFS  recursion</t>
+  </si>
+  <si>
+    <t>Trees ( Advance )</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>DFS,recursion</t>
   </si>
 </sst>
 </file>
@@ -1588,10 +1597,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2358,6 +2367,28 @@
         <v>45782</v>
       </c>
     </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>93</v>
+      </c>
+      <c r="E89" s="13">
+        <v>45784</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
102. Binary Tree Level Order Traversal (Level order traversal)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>Q No.</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>DFS,recursion</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>BFS,level order traversal</t>
   </si>
 </sst>
 </file>
@@ -1597,10 +1603,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2389,6 +2395,23 @@
         <v>45784</v>
       </c>
     </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>102</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" s="13">
+        <v>45785</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
200. Number of Islands
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
   <si>
     <t>Q No.</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>Graph , Adjacency List , DFS</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t>Graph , BFS , queue ,counting</t>
   </si>
 </sst>
 </file>
@@ -1621,10 +1627,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2474,6 +2480,23 @@
         <v>45791</v>
       </c>
     </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>200</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D99" t="s">
+        <v>103</v>
+      </c>
+      <c r="E99" s="13">
+        <v>45806</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2359. Find Closest Node to Given Two Nodes (graph-distance)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="106">
   <si>
     <t>Q No.</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>Graph , BFS , queue ,counting</t>
+  </si>
+  <si>
+    <t>Find Closest Node to Given Two Nodes</t>
+  </si>
+  <si>
+    <t>Directed graph,DFS ,Hashmap , distance calculation</t>
   </si>
 </sst>
 </file>
@@ -1627,10 +1633,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2497,6 +2503,23 @@
         <v>45806</v>
       </c>
     </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>2359</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" t="s">
+        <v>105</v>
+      </c>
+      <c r="E100" s="13">
+        <v>45807</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
909. Snakes and Ladders
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
   <si>
     <t>Q No.</t>
   </si>
@@ -119,6 +119,12 @@
     <t>Max Sum of a Pair With Equal Sum of Digits</t>
   </si>
   <si>
+    <t>Snakes and Ladders</t>
+  </si>
+  <si>
+    <t>Array , BFS ,Matrix</t>
+  </si>
+  <si>
     <t>Two pointers (Basics)</t>
   </si>
   <si>
@@ -345,6 +351,18 @@
   </si>
   <si>
     <t>Directed graph,DFS ,Hashmap , distance calculation</t>
+  </si>
+  <si>
+    <t>Total Question Solved:</t>
+  </si>
+  <si>
+    <t>Easy Questions :</t>
+  </si>
+  <si>
+    <t>Medium Questions:</t>
+  </si>
+  <si>
+    <t>Hard Questions:</t>
   </si>
 </sst>
 </file>
@@ -358,7 +376,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,21 +408,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="5" tint="-0.25"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="5" tint="-0.25"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -432,13 +450,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -583,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +622,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFD9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE7455"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6BD91"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,137 +974,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1073,10 +1126,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1097,8 +1153,29 @@
     <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1367,6 +1444,13 @@
       <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="00FAFD9B"/>
+      <color rgb="00EE7455"/>
+      <color rgb="00E6BD91"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1633,15 +1717,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.890625" customWidth="1"/>
+    <col min="1" max="1" width="15.1015625" customWidth="1"/>
     <col min="2" max="2" width="61.453125" customWidth="1"/>
     <col min="3" max="3" width="14.328125" customWidth="1"/>
     <col min="4" max="4" width="42.3203125" customWidth="1"/>
@@ -1674,7 +1758,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1689,7 +1773,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>45688</v>
       </c>
     </row>
@@ -1706,7 +1790,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="14">
         <v>45688</v>
       </c>
     </row>
@@ -1723,7 +1807,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="14">
         <v>45689</v>
       </c>
     </row>
@@ -1740,7 +1824,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="14">
         <v>45689</v>
       </c>
     </row>
@@ -1757,7 +1841,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="14">
         <v>45690</v>
       </c>
     </row>
@@ -1774,7 +1858,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="14">
         <v>45691</v>
       </c>
     </row>
@@ -1791,7 +1875,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="14">
         <v>45692</v>
       </c>
     </row>
@@ -1808,7 +1892,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="14">
         <v>45693</v>
       </c>
     </row>
@@ -1830,7 +1914,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="14">
         <v>45691</v>
       </c>
     </row>
@@ -1847,7 +1931,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="14">
         <v>45692</v>
       </c>
     </row>
@@ -1864,7 +1948,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="14">
         <v>45694</v>
       </c>
     </row>
@@ -1881,7 +1965,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="14">
         <v>45697</v>
       </c>
     </row>
@@ -1898,74 +1982,74 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="14">
         <v>45700</v>
       </c>
     </row>
-    <row r="22" ht="25" customHeight="1" spans="2:2">
-      <c r="B22" s="4" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>909</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>125</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E21" s="14">
+        <v>45808</v>
+      </c>
+    </row>
+    <row r="23" ht="25" customHeight="1" spans="2:2">
+      <c r="B23" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E24" s="13">
-        <v>45693</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="14">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>167</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="14">
         <v>45694</v>
       </c>
     </row>
-    <row r="27" ht="31" customHeight="1" spans="2:2">
-      <c r="B27" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>11</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="28" ht="31" customHeight="1" spans="2:2">
+      <c r="B28" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E29" s="13">
-        <v>45695</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>38</v>
@@ -1976,15 +2060,15 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="13">
-        <v>45699</v>
+      <c r="E30" s="14">
+        <v>45695</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>763</v>
-      </c>
-      <c r="B31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C31" t="s">
@@ -1993,35 +2077,38 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="14">
+        <v>45699</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>763</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="14">
         <v>45746</v>
       </c>
     </row>
-    <row r="33" ht="32" customHeight="1" spans="2:2">
-      <c r="B33" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" t="s">
+    <row r="34" ht="32" customHeight="1" spans="2:2">
+      <c r="B34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="13">
-        <v>45700</v>
-      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>567</v>
+        <v>3</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>45</v>
@@ -2032,41 +2119,41 @@
       <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="14">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>567</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="14">
         <v>45701</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="5"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" ht="39" customHeight="1" spans="2:2">
-      <c r="B38" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" ht="17" spans="1:5">
-      <c r="A40">
+    <row r="38" spans="2:5">
+      <c r="B38" s="8"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" ht="39" customHeight="1" spans="2:2">
+      <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" ht="17" spans="1:5">
+      <c r="A41">
         <v>424</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="13">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
-        <v>2799</v>
-      </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C41" t="s">
@@ -2075,15 +2162,15 @@
       <c r="D41" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="13">
-        <v>45771</v>
+      <c r="E41" s="14">
+        <v>45716</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>2962</v>
-      </c>
-      <c r="B42" s="7" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C42" t="s">
@@ -2092,137 +2179,137 @@
       <c r="D42" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="14">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>2962</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="14">
         <v>45776</v>
       </c>
     </row>
-    <row r="44" ht="31" customHeight="1" spans="2:2">
-      <c r="B44" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46">
+    <row r="45" ht="31" customHeight="1" spans="2:2">
+      <c r="B45" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
         <v>3066</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
         <v>22</v>
       </c>
-      <c r="D46" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="13">
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="14">
         <v>45701</v>
       </c>
     </row>
-    <row r="48" ht="38" customHeight="1" spans="2:2">
-      <c r="B48" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50">
-        <v>20</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" t="s">
+    <row r="49" ht="38" customHeight="1" spans="2:2">
+      <c r="B49" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="E50" s="13">
-        <v>45719</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
-        <v>155</v>
-      </c>
-      <c r="B51" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D51" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="14">
+        <v>45719</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>155</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="14">
         <v>45731</v>
       </c>
     </row>
-    <row r="53" ht="40" customHeight="1" spans="2:2">
-      <c r="B53" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55">
+    <row r="54" ht="40" customHeight="1" spans="2:2">
+      <c r="B54" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
         <v>739</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B56" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
         <v>22</v>
       </c>
-      <c r="D55" t="s">
-        <v>64</v>
-      </c>
-      <c r="E55" s="13">
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="14">
         <v>45732</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="1" spans="1:5">
-      <c r="A56" s="1">
+    <row r="57" s="1" customFormat="1" spans="1:5">
+      <c r="A57" s="1">
         <v>84</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B57" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E56" s="14">
+      <c r="E57" s="15">
         <v>45745</v>
       </c>
     </row>
-    <row r="59" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B59" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" customFormat="1" ht="18" spans="1:5">
-      <c r="A61">
+    <row r="60" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B60" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" customFormat="1" ht="18" spans="1:5">
+      <c r="A62">
         <v>206</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" t="s">
-        <v>69</v>
-      </c>
-      <c r="E61" s="13">
-        <v>45746</v>
-      </c>
-    </row>
-    <row r="62" customFormat="1" spans="1:5">
-      <c r="A62">
-        <v>21</v>
-      </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C62" t="s">
@@ -2231,167 +2318,167 @@
       <c r="D62" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="13">
+      <c r="E62" s="14">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="63" customFormat="1" spans="1:5">
+      <c r="A63">
+        <v>21</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" s="14">
         <v>45747</v>
       </c>
     </row>
-    <row r="63" customFormat="1" spans="5:5">
-      <c r="E63" s="13"/>
-    </row>
-    <row r="64" customFormat="1" spans="2:5">
-      <c r="B64" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" customFormat="1" spans="5:5">
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" customFormat="1" spans="1:5">
-      <c r="A66">
-        <v>2</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66" s="13">
-        <v>45747</v>
-      </c>
+    <row r="64" customFormat="1" spans="5:5">
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" customFormat="1" spans="2:5">
+      <c r="B65" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" customFormat="1" spans="5:5">
+      <c r="E66" s="14"/>
     </row>
     <row r="67" customFormat="1" spans="1:5">
       <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" s="14">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" spans="1:5">
+      <c r="A68">
         <v>141</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" t="s">
         <v>7</v>
       </c>
-      <c r="D67" t="s">
-        <v>75</v>
-      </c>
-      <c r="E67" s="13">
+      <c r="D68" t="s">
+        <v>77</v>
+      </c>
+      <c r="E68" s="14">
         <v>45748</v>
       </c>
     </row>
-    <row r="69" ht="35" customHeight="1" spans="2:2">
-      <c r="B69" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71">
+    <row r="70" ht="35" customHeight="1" spans="2:2">
+      <c r="B70" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
         <v>226</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B72" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" t="s">
         <v>7</v>
       </c>
-      <c r="D71" t="s">
-        <v>78</v>
-      </c>
-      <c r="E71" s="13">
+      <c r="D72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E72" s="14">
         <v>45733</v>
       </c>
     </row>
-    <row r="73" ht="39" customHeight="1" spans="2:2">
-      <c r="B73" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75">
-        <v>704</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" t="s">
+    <row r="74" ht="39" customHeight="1" spans="2:2">
+      <c r="B74" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="E75" s="13">
-        <v>45757</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76">
-        <v>33</v>
-      </c>
-      <c r="B76" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
         <v>83</v>
       </c>
-      <c r="E76" s="13">
+      <c r="E76" s="14">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>33</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" t="s">
+        <v>85</v>
+      </c>
+      <c r="E77" s="14">
         <v>45759</v>
       </c>
     </row>
-    <row r="78" ht="32" customHeight="1" spans="2:2">
-      <c r="B78" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" ht="30" customHeight="1" spans="1:5">
-      <c r="A80">
+    <row r="79" ht="32" customHeight="1" spans="2:2">
+      <c r="B79" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" ht="30" customHeight="1" spans="1:5">
+      <c r="A81">
         <v>34</v>
       </c>
-      <c r="B80" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="B81" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" t="s">
         <v>22</v>
       </c>
-      <c r="D80" t="s">
-        <v>86</v>
-      </c>
-      <c r="E80" s="13">
+      <c r="D81" t="s">
+        <v>88</v>
+      </c>
+      <c r="E81" s="14">
         <v>45773</v>
       </c>
     </row>
-    <row r="82" ht="29" customHeight="1" spans="2:2">
-      <c r="B82" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84">
-        <v>226</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C84" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" t="s">
-        <v>88</v>
-      </c>
-      <c r="E84" s="13">
-        <v>45774</v>
+    <row r="83" ht="29" customHeight="1" spans="2:2">
+      <c r="B83" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85">
-        <v>104</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>89</v>
+        <v>226</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -2399,98 +2486,98 @@
       <c r="D85" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="13">
+      <c r="E85" s="14">
+        <v>45774</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>104</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>92</v>
+      </c>
+      <c r="E86" s="14">
         <v>45782</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
-      <c r="B87" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89">
-        <v>100</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" t="s">
+    <row r="88" spans="2:2">
+      <c r="B88" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="E89" s="13">
-        <v>45784</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90">
-        <v>102</v>
-      </c>
-      <c r="B90" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D90" t="s">
         <v>95</v>
       </c>
-      <c r="E90" s="13">
+      <c r="E90" s="14">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>102</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91" t="s">
+        <v>22</v>
+      </c>
+      <c r="D91" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" s="14">
         <v>45785</v>
       </c>
     </row>
-    <row r="92" ht="27" customHeight="1" spans="2:2">
-      <c r="B92" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94">
+    <row r="93" ht="27" customHeight="1" spans="2:2">
+      <c r="B93" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
         <v>235</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="B95" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95" t="s">
         <v>22</v>
       </c>
-      <c r="D94" t="s">
-        <v>98</v>
-      </c>
-      <c r="E94" s="13">
+      <c r="D95" t="s">
+        <v>100</v>
+      </c>
+      <c r="E95" s="14">
         <v>45786</v>
       </c>
     </row>
-    <row r="96" ht="24" customHeight="1" spans="2:2">
-      <c r="B96" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98">
-        <v>133</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C98" t="s">
-        <v>22</v>
-      </c>
-      <c r="D98" t="s">
+    <row r="97" ht="24" customHeight="1" spans="2:2">
+      <c r="B97" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="E98" s="13">
-        <v>45791</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99">
-        <v>200</v>
-      </c>
-      <c r="B99" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C99" t="s">
@@ -2499,15 +2586,15 @@
       <c r="D99" t="s">
         <v>103</v>
       </c>
-      <c r="E99" s="13">
-        <v>45806</v>
+      <c r="E99" s="14">
+        <v>45791</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100">
-        <v>2359</v>
-      </c>
-      <c r="B100" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C100" t="s">
@@ -2516,8 +2603,61 @@
       <c r="D100" t="s">
         <v>105</v>
       </c>
-      <c r="E100" s="13">
+      <c r="E100" s="14">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>2359</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
+        <v>107</v>
+      </c>
+      <c r="E101" s="14">
         <v>45807</v>
+      </c>
+    </row>
+    <row r="106" ht="41" customHeight="1" spans="1:2">
+      <c r="A106" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" s="17">
+        <f>COUNT(A:A)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" ht="30" customHeight="1" spans="1:2">
+      <c r="A108" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="19">
+        <f>COUNTIF(C:C,"Easy")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" ht="40" customHeight="1" spans="1:2">
+      <c r="A109" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" s="21">
+        <f>COUNTIF(C:C,"Medium")</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="110" ht="36" customHeight="1" spans="1:2">
+      <c r="A110" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" s="23">
+        <f>COUNTIF(C:C,"Hard")</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4. Median of Two Sorted Arrays (sorting)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
   <si>
     <t>Q No.</t>
   </si>
@@ -351,6 +351,15 @@
   </si>
   <si>
     <t>Directed graph,DFS ,Hashmap , distance calculation</t>
+  </si>
+  <si>
+    <t>Graphs (advanced - Union Find)</t>
+  </si>
+  <si>
+    <t>Lexicographically Smallest Equivalent String</t>
+  </si>
+  <si>
+    <t>Union Find ,Graph</t>
   </si>
   <si>
     <t>Total Question Solved:</t>
@@ -1104,7 +1113,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1125,9 +1134,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1717,10 +1723,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1758,7 +1764,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -1773,7 +1779,7 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>45688</v>
       </c>
     </row>
@@ -1790,7 +1796,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>45688</v>
       </c>
     </row>
@@ -1807,7 +1813,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>45689</v>
       </c>
     </row>
@@ -1824,7 +1830,7 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>45689</v>
       </c>
     </row>
@@ -1841,7 +1847,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>45690</v>
       </c>
     </row>
@@ -1858,7 +1864,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>45691</v>
       </c>
     </row>
@@ -1875,7 +1881,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>45692</v>
       </c>
     </row>
@@ -1892,7 +1898,7 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>45693</v>
       </c>
     </row>
@@ -1914,7 +1920,7 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>45691</v>
       </c>
     </row>
@@ -1931,7 +1937,7 @@
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>45692</v>
       </c>
     </row>
@@ -1948,7 +1954,7 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>45694</v>
       </c>
     </row>
@@ -1965,7 +1971,7 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>45697</v>
       </c>
     </row>
@@ -1982,7 +1988,7 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>45700</v>
       </c>
     </row>
@@ -1999,7 +2005,7 @@
       <c r="D21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <v>45808</v>
       </c>
     </row>
@@ -2021,7 +2027,7 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <v>45693</v>
       </c>
     </row>
@@ -2038,7 +2044,7 @@
       <c r="D26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <v>45694</v>
       </c>
     </row>
@@ -2060,7 +2066,7 @@
       <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="13">
         <v>45695</v>
       </c>
     </row>
@@ -2077,7 +2083,7 @@
       <c r="D31" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="13">
         <v>45699</v>
       </c>
     </row>
@@ -2094,7 +2100,7 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="13">
         <v>45746</v>
       </c>
     </row>
@@ -2104,7 +2110,7 @@
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="7"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
@@ -2119,7 +2125,7 @@
       <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="13">
         <v>45700</v>
       </c>
     </row>
@@ -2136,13 +2142,13 @@
       <c r="D37" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="13">
         <v>45701</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="8"/>
-      <c r="E38" s="14"/>
+      <c r="B38" s="7"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" ht="39" customHeight="1" spans="2:2">
       <c r="B39" s="4" t="s">
@@ -2153,7 +2159,7 @@
       <c r="A41">
         <v>424</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C41" t="s">
@@ -2162,7 +2168,7 @@
       <c r="D41" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="13">
         <v>45716</v>
       </c>
     </row>
@@ -2179,7 +2185,7 @@
       <c r="D42" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="13">
         <v>45771</v>
       </c>
     </row>
@@ -2196,12 +2202,12 @@
       <c r="D43" t="s">
         <v>55</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="13">
         <v>45776</v>
       </c>
     </row>
     <row r="45" ht="31" customHeight="1" spans="2:2">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2218,12 +2224,12 @@
       <c r="D47" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="13">
         <v>45701</v>
       </c>
     </row>
     <row r="49" ht="38" customHeight="1" spans="2:2">
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2240,7 +2246,7 @@
       <c r="D51" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="13">
         <v>45719</v>
       </c>
     </row>
@@ -2257,12 +2263,12 @@
       <c r="D52" t="s">
         <v>63</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="13">
         <v>45731</v>
       </c>
     </row>
     <row r="54" ht="40" customHeight="1" spans="2:2">
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2279,7 +2285,7 @@
       <c r="D56" t="s">
         <v>66</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="13">
         <v>45732</v>
       </c>
     </row>
@@ -2287,7 +2293,7 @@
       <c r="A57" s="1">
         <v>84</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2296,7 +2302,7 @@
       <c r="D57" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="14">
         <v>45745</v>
       </c>
     </row>
@@ -2309,7 +2315,7 @@
       <c r="A62">
         <v>206</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C62" t="s">
@@ -2318,7 +2324,7 @@
       <c r="D62" t="s">
         <v>71</v>
       </c>
-      <c r="E62" s="14">
+      <c r="E62" s="13">
         <v>45746</v>
       </c>
     </row>
@@ -2335,21 +2341,21 @@
       <c r="D63" t="s">
         <v>73</v>
       </c>
-      <c r="E63" s="14">
+      <c r="E63" s="13">
         <v>45747</v>
       </c>
     </row>
     <row r="64" customFormat="1" spans="5:5">
-      <c r="E64" s="14"/>
+      <c r="E64" s="13"/>
     </row>
     <row r="65" customFormat="1" spans="2:5">
       <c r="B65" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E65" s="14"/>
+      <c r="E65" s="13"/>
     </row>
     <row r="66" customFormat="1" spans="5:5">
-      <c r="E66" s="14"/>
+      <c r="E66" s="13"/>
     </row>
     <row r="67" customFormat="1" spans="1:5">
       <c r="A67">
@@ -2364,7 +2370,7 @@
       <c r="D67" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="14">
+      <c r="E67" s="13">
         <v>45747</v>
       </c>
     </row>
@@ -2381,12 +2387,12 @@
       <c r="D68" t="s">
         <v>77</v>
       </c>
-      <c r="E68" s="14">
+      <c r="E68" s="13">
         <v>45748</v>
       </c>
     </row>
     <row r="70" ht="35" customHeight="1" spans="2:2">
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2403,12 +2409,12 @@
       <c r="D72" t="s">
         <v>80</v>
       </c>
-      <c r="E72" s="14">
+      <c r="E72" s="13">
         <v>45733</v>
       </c>
     </row>
     <row r="74" ht="39" customHeight="1" spans="2:2">
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2425,7 +2431,7 @@
       <c r="D76" t="s">
         <v>83</v>
       </c>
-      <c r="E76" s="14">
+      <c r="E76" s="13">
         <v>45757</v>
       </c>
     </row>
@@ -2442,12 +2448,12 @@
       <c r="D77" t="s">
         <v>85</v>
       </c>
-      <c r="E77" s="14">
+      <c r="E77" s="13">
         <v>45759</v>
       </c>
     </row>
     <row r="79" ht="32" customHeight="1" spans="2:2">
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="9" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2464,12 +2470,12 @@
       <c r="D81" t="s">
         <v>88</v>
       </c>
-      <c r="E81" s="14">
+      <c r="E81" s="13">
         <v>45773</v>
       </c>
     </row>
     <row r="83" ht="29" customHeight="1" spans="2:2">
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2486,7 +2492,7 @@
       <c r="D85" t="s">
         <v>90</v>
       </c>
-      <c r="E85" s="14">
+      <c r="E85" s="13">
         <v>45774</v>
       </c>
     </row>
@@ -2503,12 +2509,12 @@
       <c r="D86" t="s">
         <v>92</v>
       </c>
-      <c r="E86" s="14">
+      <c r="E86" s="13">
         <v>45782</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2525,7 +2531,7 @@
       <c r="D90" t="s">
         <v>95</v>
       </c>
-      <c r="E90" s="14">
+      <c r="E90" s="13">
         <v>45784</v>
       </c>
     </row>
@@ -2542,12 +2548,12 @@
       <c r="D91" t="s">
         <v>97</v>
       </c>
-      <c r="E91" s="14">
+      <c r="E91" s="13">
         <v>45785</v>
       </c>
     </row>
     <row r="93" ht="27" customHeight="1" spans="2:2">
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2564,7 +2570,7 @@
       <c r="D95" t="s">
         <v>100</v>
       </c>
-      <c r="E95" s="14">
+      <c r="E95" s="13">
         <v>45786</v>
       </c>
     </row>
@@ -2586,7 +2592,7 @@
       <c r="D99" t="s">
         <v>103</v>
       </c>
-      <c r="E99" s="14">
+      <c r="E99" s="13">
         <v>45791</v>
       </c>
     </row>
@@ -2603,7 +2609,7 @@
       <c r="D100" t="s">
         <v>105</v>
       </c>
-      <c r="E100" s="14">
+      <c r="E100" s="13">
         <v>45806</v>
       </c>
     </row>
@@ -2620,42 +2626,64 @@
       <c r="D101" t="s">
         <v>107</v>
       </c>
-      <c r="E101" s="14">
+      <c r="E101" s="13">
         <v>45807</v>
       </c>
     </row>
-    <row r="106" ht="41" customHeight="1" spans="1:2">
-      <c r="A106" s="16" t="s">
+    <row r="103" ht="29" customHeight="1" spans="2:2">
+      <c r="B103" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B106" s="17">
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105">
+        <v>106</v>
+      </c>
+      <c r="B105" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" t="s">
+        <v>110</v>
+      </c>
+      <c r="E105" s="13">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="116" ht="41" customHeight="1" spans="1:2">
+      <c r="A116" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116" s="16">
         <f>COUNT(A:A)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="108" ht="30" customHeight="1" spans="1:2">
-      <c r="A108" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B108" s="19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" ht="30" customHeight="1" spans="1:2">
+      <c r="A118" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="18">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>18</v>
       </c>
     </row>
-    <row r="109" ht="40" customHeight="1" spans="1:2">
-      <c r="A109" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B109" s="21">
+    <row r="119" ht="40" customHeight="1" spans="1:2">
+      <c r="A119" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B119" s="20">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="110" ht="36" customHeight="1" spans="1:2">
-      <c r="A110" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B110" s="23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" ht="36" customHeight="1" spans="1:2">
+      <c r="A120" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B120" s="22">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
207. Course Schedule (cycle detection + dfs)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="117">
   <si>
     <t>Q No.</t>
   </si>
@@ -353,13 +353,19 @@
     <t>Directed graph,DFS ,Hashmap , distance calculation</t>
   </si>
   <si>
-    <t>Graphs (advanced - Union Find)</t>
+    <t>Graphs (advanced)</t>
   </si>
   <si>
     <t>Lexicographically Smallest Equivalent String</t>
   </si>
   <si>
     <t>Union Find ,Graph</t>
+  </si>
+  <si>
+    <t>Course Schedule</t>
+  </si>
+  <si>
+    <t>DFS , Topological Sort ,Cycle detection</t>
   </si>
   <si>
     <t>Total Question Solved:</t>
@@ -1725,8 +1731,8 @@
   <sheetPr/>
   <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -2652,18 +2658,35 @@
         <v>45782</v>
       </c>
     </row>
+    <row r="106" spans="1:5">
+      <c r="A106">
+        <v>207</v>
+      </c>
+      <c r="B106" t="s">
+        <v>111</v>
+      </c>
+      <c r="C106" t="s">
+        <v>22</v>
+      </c>
+      <c r="D106" t="s">
+        <v>112</v>
+      </c>
+      <c r="E106" s="13">
+        <v>45817</v>
+      </c>
+    </row>
     <row r="116" ht="41" customHeight="1" spans="1:2">
       <c r="A116" s="15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B116" s="16">
         <f>COUNT(A:A)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="118" ht="30" customHeight="1" spans="1:2">
       <c r="A118" s="17" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B118" s="18">
         <f>COUNTIF(C:C,"Easy")</f>
@@ -2672,16 +2695,16 @@
     </row>
     <row r="119" ht="40" customHeight="1" spans="1:2">
       <c r="A119" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B119" s="20">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" ht="36" customHeight="1" spans="1:2">
       <c r="A120" s="21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B120" s="22">
         <f>COUNTIF(C:C,"Hard")</f>

</xml_diff>

<commit_message>
2966. Divide Array Into Arrays With Max Difference (Sliding window)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="122">
   <si>
     <t>Q No.</t>
   </si>
@@ -44,6 +44,9 @@
     <t>Date solved</t>
   </si>
   <si>
+    <t>Language</t>
+  </si>
+  <si>
     <t>Arrays (Basics)</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
     <t>Arrays</t>
   </si>
   <si>
+    <t>Python</t>
+  </si>
+  <si>
     <t>Best Time to Buy and Sell Stock</t>
   </si>
   <si>
@@ -138,6 +144,15 @@
   </si>
   <si>
     <t>Arrays,Two pointers,Binary Search</t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>Arrays , Two pointer</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
   <si>
     <t>Two pointers (Advance)</t>
@@ -1729,13 +1744,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="15.1015625" customWidth="1"/>
     <col min="2" max="2" width="61.453125" customWidth="1"/>
@@ -1744,7 +1759,7 @@
     <col min="5" max="5" width="13.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="39" customHeight="1" spans="1:5">
+    <row r="1" ht="39" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1760,953 +1775,1117 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="12">
         <v>45688</v>
       </c>
-    </row>
-    <row r="6" ht="18" spans="1:5">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="18" spans="1:6">
       <c r="A6">
         <v>121</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
       </c>
       <c r="E6" s="13">
         <v>45688</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>3151</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E7" s="13">
         <v>45689</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>242</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" s="13">
         <v>45689</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1752</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="13">
         <v>45690</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>3105</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="13">
         <v>45691</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1800</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="13">
         <v>45692</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1790</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12" s="13">
         <v>45693</v>
       </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" ht="30" customHeight="1" spans="2:2">
       <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>238</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E16" s="13">
         <v>45691</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>347</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E17" s="13">
         <v>45692</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>1726</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E18" s="13">
         <v>45694</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>2364</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E19" s="13">
         <v>45697</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>2342</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E20" s="13">
         <v>45700</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>909</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E21" s="13">
         <v>45808</v>
       </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" ht="25" customHeight="1" spans="2:2">
       <c r="B23" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>125</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E25" s="13">
         <v>45693</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>167</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E26" s="13">
         <v>45694</v>
       </c>
-    </row>
-    <row r="28" ht="31" customHeight="1" spans="2:2">
-      <c r="B28" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>283</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="13">
+        <v>45826</v>
+      </c>
+      <c r="F27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" ht="31" customHeight="1" spans="2:2">
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
         <v>11</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="13">
+      <c r="B31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="13">
         <v>45695</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
         <v>15</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="13">
+      <c r="B32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="13">
         <v>45699</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
         <v>763</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="13">
+      <c r="B33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="13">
         <v>45746</v>
       </c>
-    </row>
-    <row r="34" ht="32" customHeight="1" spans="2:2">
-      <c r="B34" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36">
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" ht="32" customHeight="1" spans="2:2">
+      <c r="B35" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
         <v>3</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="13">
+      <c r="B37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="13">
         <v>45700</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37">
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
         <v>567</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="13">
+        <v>45701</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="7"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" ht="39" customHeight="1" spans="2:2">
+      <c r="B40" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" ht="17" spans="1:6">
+      <c r="A42">
+        <v>424</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="13">
+        <v>45716</v>
+      </c>
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>2799</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="13">
+        <v>45771</v>
+      </c>
+      <c r="F43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>2962</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="13">
+        <v>45776</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" ht="31" customHeight="1" spans="2:2">
+      <c r="B46" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>3066</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="13">
+        <v>45701</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" ht="38" customHeight="1" spans="2:2">
+      <c r="B50" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="13">
+        <v>45719</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>155</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="13">
+        <v>45731</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" ht="40" customHeight="1" spans="2:2">
+      <c r="B55" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>739</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="13">
+        <v>45732</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" s="1" customFormat="1" spans="1:6">
+      <c r="A58" s="1">
+        <v>84</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="14">
+        <v>45745</v>
+      </c>
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B61" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" customFormat="1" ht="18" spans="1:6">
+      <c r="A63">
+        <v>206</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="13">
+        <v>45746</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" customFormat="1" spans="1:6">
+      <c r="A64">
+        <v>21</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>78</v>
+      </c>
+      <c r="E64" s="13">
+        <v>45747</v>
+      </c>
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" spans="5:5">
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" customFormat="1" spans="2:5">
+      <c r="B66" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" customFormat="1" spans="5:5">
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" customFormat="1" spans="1:6">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" t="s">
+        <v>78</v>
+      </c>
+      <c r="E68" s="13">
+        <v>45747</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" customFormat="1" spans="1:6">
+      <c r="A69">
+        <v>141</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69" s="13">
+        <v>45748</v>
+      </c>
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" ht="35" customHeight="1" spans="2:2">
+      <c r="B71" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>226</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>85</v>
+      </c>
+      <c r="E73" s="13">
+        <v>45733</v>
+      </c>
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" ht="39" customHeight="1" spans="2:2">
+      <c r="B75" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>704</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>88</v>
+      </c>
+      <c r="E77" s="13">
+        <v>45757</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>33</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="13">
+        <v>45759</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" ht="32" customHeight="1" spans="2:2">
+      <c r="B80" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" ht="30" customHeight="1" spans="1:6">
+      <c r="A82">
+        <v>34</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" t="s">
+        <v>93</v>
+      </c>
+      <c r="E82" s="13">
+        <v>45773</v>
+      </c>
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" ht="29" customHeight="1" spans="2:2">
+      <c r="B84" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>226</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>95</v>
+      </c>
+      <c r="E86" s="13">
+        <v>45774</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <v>104</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>97</v>
+      </c>
+      <c r="E87" s="13">
+        <v>45782</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>100</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>100</v>
+      </c>
+      <c r="E91" s="13">
+        <v>45784</v>
+      </c>
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>102</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92" s="13">
+        <v>45785</v>
+      </c>
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" ht="27" customHeight="1" spans="2:2">
+      <c r="B94" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>235</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" t="s">
+        <v>105</v>
+      </c>
+      <c r="E96" s="13">
+        <v>45786</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" ht="24" customHeight="1" spans="2:2">
+      <c r="B98" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>133</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" t="s">
+        <v>108</v>
+      </c>
+      <c r="E100" s="13">
+        <v>45791</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>200</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" t="s">
+        <v>110</v>
+      </c>
+      <c r="E101" s="13">
+        <v>45806</v>
+      </c>
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>2359</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C102" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" s="13">
+        <v>45807</v>
+      </c>
+      <c r="F102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" ht="29" customHeight="1" spans="2:2">
+      <c r="B104" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>114</v>
+      </c>
+      <c r="C106" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" t="s">
+        <v>115</v>
+      </c>
+      <c r="E106" s="13">
+        <v>45782</v>
+      </c>
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>207</v>
+      </c>
+      <c r="B107" t="s">
+        <v>116</v>
+      </c>
+      <c r="C107" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" t="s">
+        <v>117</v>
+      </c>
+      <c r="E107" s="13">
+        <v>45817</v>
+      </c>
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" ht="41" customHeight="1" spans="1:2">
+      <c r="A117" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117" s="16">
+        <f>COUNT(A:A)</f>
         <v>48</v>
       </c>
-      <c r="E37" s="13">
-        <v>45701</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="7"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" ht="39" customHeight="1" spans="2:2">
-      <c r="B39" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" ht="17" spans="1:5">
-      <c r="A41">
-        <v>424</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="13">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42">
-        <v>2799</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="13">
-        <v>45771</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43">
-        <v>2962</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="13">
-        <v>45776</v>
-      </c>
-    </row>
-    <row r="45" ht="31" customHeight="1" spans="2:2">
-      <c r="B45" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47">
-        <v>3066</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" t="s">
-        <v>58</v>
-      </c>
-      <c r="E47" s="13">
-        <v>45701</v>
-      </c>
-    </row>
-    <row r="49" ht="38" customHeight="1" spans="2:2">
-      <c r="B49" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51">
-        <v>20</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="13">
-        <v>45719</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52">
-        <v>155</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" s="13">
-        <v>45731</v>
-      </c>
-    </row>
-    <row r="54" ht="40" customHeight="1" spans="2:2">
-      <c r="B54" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56">
-        <v>739</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" t="s">
-        <v>66</v>
-      </c>
-      <c r="E56" s="13">
-        <v>45732</v>
-      </c>
-    </row>
-    <row r="57" s="1" customFormat="1" spans="1:5">
-      <c r="A57" s="1">
-        <v>84</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E57" s="14">
-        <v>45745</v>
-      </c>
-    </row>
-    <row r="60" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B60" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="62" customFormat="1" ht="18" spans="1:5">
-      <c r="A62">
-        <v>206</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" t="s">
-        <v>71</v>
-      </c>
-      <c r="E62" s="13">
-        <v>45746</v>
-      </c>
-    </row>
-    <row r="63" customFormat="1" spans="1:5">
-      <c r="A63">
-        <v>21</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" t="s">
-        <v>73</v>
-      </c>
-      <c r="E63" s="13">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="64" customFormat="1" spans="5:5">
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" customFormat="1" spans="2:5">
-      <c r="B65" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" customFormat="1" spans="5:5">
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" customFormat="1" spans="1:5">
-      <c r="A67">
-        <v>2</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C67" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" s="13">
-        <v>45747</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" spans="1:5">
-      <c r="A68">
-        <v>141</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C68" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" t="s">
-        <v>77</v>
-      </c>
-      <c r="E68" s="13">
-        <v>45748</v>
-      </c>
-    </row>
-    <row r="70" ht="35" customHeight="1" spans="2:2">
-      <c r="B70" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72">
-        <v>226</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" s="13">
-        <v>45733</v>
-      </c>
-    </row>
-    <row r="74" ht="39" customHeight="1" spans="2:2">
-      <c r="B74" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76">
-        <v>704</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" t="s">
-        <v>83</v>
-      </c>
-      <c r="E76" s="13">
-        <v>45757</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77">
-        <v>33</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C77" t="s">
-        <v>22</v>
-      </c>
-      <c r="D77" t="s">
-        <v>85</v>
-      </c>
-      <c r="E77" s="13">
-        <v>45759</v>
-      </c>
-    </row>
-    <row r="79" ht="32" customHeight="1" spans="2:2">
-      <c r="B79" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" ht="30" customHeight="1" spans="1:5">
-      <c r="A81">
-        <v>34</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C81" t="s">
-        <v>22</v>
-      </c>
-      <c r="D81" t="s">
-        <v>88</v>
-      </c>
-      <c r="E81" s="13">
-        <v>45773</v>
-      </c>
-    </row>
-    <row r="83" ht="29" customHeight="1" spans="2:2">
-      <c r="B83" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85">
-        <v>226</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C85" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" t="s">
-        <v>90</v>
-      </c>
-      <c r="E85" s="13">
-        <v>45774</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86">
-        <v>104</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" t="s">
-        <v>92</v>
-      </c>
-      <c r="E86" s="13">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2">
-      <c r="B88" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90">
-        <v>100</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" t="s">
-        <v>95</v>
-      </c>
-      <c r="E90" s="13">
-        <v>45784</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91">
-        <v>102</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C91" t="s">
-        <v>22</v>
-      </c>
-      <c r="D91" t="s">
-        <v>97</v>
-      </c>
-      <c r="E91" s="13">
-        <v>45785</v>
-      </c>
-    </row>
-    <row r="93" ht="27" customHeight="1" spans="2:2">
-      <c r="B93" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95">
-        <v>235</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C95" t="s">
-        <v>22</v>
-      </c>
-      <c r="D95" t="s">
-        <v>100</v>
-      </c>
-      <c r="E95" s="13">
-        <v>45786</v>
-      </c>
-    </row>
-    <row r="97" ht="24" customHeight="1" spans="2:2">
-      <c r="B97" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99">
-        <v>133</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C99" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" t="s">
-        <v>103</v>
-      </c>
-      <c r="E99" s="13">
-        <v>45791</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100">
-        <v>200</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C100" t="s">
-        <v>22</v>
-      </c>
-      <c r="D100" t="s">
-        <v>105</v>
-      </c>
-      <c r="E100" s="13">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101">
-        <v>2359</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C101" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" t="s">
-        <v>107</v>
-      </c>
-      <c r="E101" s="13">
-        <v>45807</v>
-      </c>
-    </row>
-    <row r="103" ht="29" customHeight="1" spans="2:2">
-      <c r="B103" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105">
-        <v>106</v>
-      </c>
-      <c r="B105" t="s">
-        <v>109</v>
-      </c>
-      <c r="C105" t="s">
-        <v>22</v>
-      </c>
-      <c r="D105" t="s">
-        <v>110</v>
-      </c>
-      <c r="E105" s="13">
-        <v>45782</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106">
-        <v>207</v>
-      </c>
-      <c r="B106" t="s">
-        <v>111</v>
-      </c>
-      <c r="C106" t="s">
-        <v>22</v>
-      </c>
-      <c r="D106" t="s">
-        <v>112</v>
-      </c>
-      <c r="E106" s="13">
-        <v>45817</v>
-      </c>
-    </row>
-    <row r="116" ht="41" customHeight="1" spans="1:2">
-      <c r="A116" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B116" s="16">
-        <f>COUNT(A:A)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="118" ht="30" customHeight="1" spans="1:2">
-      <c r="A118" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B118" s="18">
+    </row>
+    <row r="119" ht="30" customHeight="1" spans="1:2">
+      <c r="A119" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="18">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="119" ht="40" customHeight="1" spans="1:2">
-      <c r="A119" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B119" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="120" ht="40" customHeight="1" spans="1:2">
+      <c r="A120" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="20">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>28</v>
       </c>
     </row>
-    <row r="120" ht="36" customHeight="1" spans="1:2">
-      <c r="A120" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B120" s="22">
+    <row r="121" ht="36" customHeight="1" spans="1:2">
+      <c r="A121" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" s="22">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
2294. Partition Array Such That Maximum Difference Is K (Two pointers)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="126">
   <si>
     <t>Q No.</t>
   </si>
@@ -155,6 +155,12 @@
     <t>Java</t>
   </si>
   <si>
+    <t>Partition Array Such That Maximum Difference Is K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrays , Two pointer ,Sorting </t>
+  </si>
+  <si>
     <t>Two pointers (Advance)</t>
   </si>
   <si>
@@ -189,6 +195,12 @@
   </si>
   <si>
     <t>String,Sliding Window,Counter</t>
+  </si>
+  <si>
+    <t>Divide Array Into Arrays With Max Difference</t>
+  </si>
+  <si>
+    <t>Array , Sliding Window</t>
   </si>
   <si>
     <t>Sliding Window (Advance)</t>
@@ -406,7 +418,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +464,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCE9178"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="5" tint="-0.25"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -468,13 +494,6 @@
       <i/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFCE9178"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1004,137 +1023,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1159,17 +1178,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1744,10 +1766,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1788,7 +1810,7 @@
       </c>
     </row>
     <row r="4" spans="5:5">
-      <c r="E4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -1803,7 +1825,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>45688</v>
       </c>
       <c r="F5" t="s">
@@ -1823,7 +1845,7 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="14">
         <v>45688</v>
       </c>
       <c r="F6" t="s">
@@ -1843,7 +1865,7 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="14">
         <v>45689</v>
       </c>
       <c r="F7" t="s">
@@ -1863,7 +1885,7 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="14">
         <v>45689</v>
       </c>
       <c r="F8" t="s">
@@ -1883,7 +1905,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="14">
         <v>45690</v>
       </c>
       <c r="F9" t="s">
@@ -1903,7 +1925,7 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="14">
         <v>45691</v>
       </c>
       <c r="F10" t="s">
@@ -1923,7 +1945,7 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="14">
         <v>45692</v>
       </c>
       <c r="F11" t="s">
@@ -1943,7 +1965,7 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="14">
         <v>45693</v>
       </c>
       <c r="F12" t="s">
@@ -1968,7 +1990,7 @@
       <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="14">
         <v>45691</v>
       </c>
       <c r="F16" t="s">
@@ -1988,7 +2010,7 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="14">
         <v>45692</v>
       </c>
       <c r="F17" t="s">
@@ -2008,7 +2030,7 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="14">
         <v>45694</v>
       </c>
       <c r="F18" t="s">
@@ -2028,7 +2050,7 @@
       <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="14">
         <v>45697</v>
       </c>
       <c r="F19" t="s">
@@ -2048,7 +2070,7 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="14">
         <v>45700</v>
       </c>
       <c r="F20" t="s">
@@ -2068,7 +2090,7 @@
       <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="14">
         <v>45808</v>
       </c>
       <c r="F21" t="s">
@@ -2093,7 +2115,7 @@
       <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="14">
         <v>45693</v>
       </c>
       <c r="F25" t="s">
@@ -2113,7 +2135,7 @@
       <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="14">
         <v>45694</v>
       </c>
       <c r="F26" t="s">
@@ -2124,7 +2146,7 @@
       <c r="A27">
         <v>283</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C27" t="s">
@@ -2133,41 +2155,41 @@
       <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="14">
         <v>45826</v>
       </c>
       <c r="F27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" ht="31" customHeight="1" spans="2:2">
-      <c r="B29" s="4" t="s">
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>2294</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E28" s="14">
+        <v>45827</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" ht="31" customHeight="1" spans="2:2">
+      <c r="B30" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="E31" s="13">
-        <v>45695</v>
-      </c>
-      <c r="F31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>45</v>
@@ -2178,8 +2200,8 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="13">
-        <v>45699</v>
+      <c r="E32" s="14">
+        <v>45695</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -2187,7 +2209,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>763</v>
+        <v>15</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>47</v>
@@ -2198,44 +2220,44 @@
       <c r="D33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="14">
+        <v>45699</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>763</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="14">
         <v>45746</v>
       </c>
-      <c r="F33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" ht="32" customHeight="1" spans="2:2">
-      <c r="B35" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>3</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" ht="32" customHeight="1" spans="2:2">
+      <c r="B36" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="13">
-        <v>45700</v>
-      </c>
-      <c r="F37" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>567</v>
+        <v>3</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>52</v>
@@ -2246,67 +2268,67 @@
       <c r="D38" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="14">
+        <v>45700</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>567</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="14">
         <v>45701</v>
       </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="7"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" ht="39" customHeight="1" spans="2:2">
-      <c r="B40" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" ht="17" spans="1:6">
-      <c r="A42">
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" ht="18" spans="1:6">
+      <c r="A40">
+        <v>2966</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="14">
+        <v>45826</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="9"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" ht="39" customHeight="1" spans="2:2">
+      <c r="B42" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" ht="17" spans="1:6">
+      <c r="A44">
         <v>424</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="13">
-        <v>45716</v>
-      </c>
-      <c r="F42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
-        <v>2799</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43" s="13">
-        <v>45771</v>
-      </c>
-      <c r="F43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
-        <v>2962</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C44" t="s">
@@ -2315,483 +2337,483 @@
       <c r="D44" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="14">
+        <v>45716</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>2799</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="14">
+        <v>45771</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>2962</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="14">
         <v>45776</v>
       </c>
-      <c r="F44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" ht="31" customHeight="1" spans="2:2">
-      <c r="B46" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48">
+      <c r="F46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" ht="31" customHeight="1" spans="2:2">
+      <c r="B48" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
         <v>3066</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B50" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D48" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" s="13">
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="14">
         <v>45701</v>
       </c>
-      <c r="F48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" ht="38" customHeight="1" spans="2:2">
-      <c r="B50" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" ht="38" customHeight="1" spans="2:2">
+      <c r="B52" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
         <v>20</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B54" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s">
         <v>8</v>
       </c>
-      <c r="D52" t="s">
-        <v>66</v>
-      </c>
-      <c r="E52" s="13">
+      <c r="D54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="14">
         <v>45719</v>
       </c>
-      <c r="F52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
         <v>155</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B55" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" t="s">
         <v>24</v>
       </c>
-      <c r="D53" t="s">
-        <v>68</v>
-      </c>
-      <c r="E53" s="13">
+      <c r="D55" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="14">
         <v>45731</v>
       </c>
-      <c r="F53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" ht="40" customHeight="1" spans="2:2">
-      <c r="B55" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" ht="40" customHeight="1" spans="2:2">
+      <c r="B57" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
         <v>739</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B59" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
         <v>24</v>
       </c>
-      <c r="D57" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" s="13">
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="14">
         <v>45732</v>
       </c>
-      <c r="F57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" s="1" customFormat="1" spans="1:6">
-      <c r="A58" s="1">
+      <c r="F59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" s="1" customFormat="1" spans="1:6">
+      <c r="A60" s="1">
         <v>84</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="14">
+      <c r="B60" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="15">
         <v>45745</v>
       </c>
-      <c r="F58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B61" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" customFormat="1" ht="18" spans="1:6">
-      <c r="A63">
+      <c r="F60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B63" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" ht="18" spans="1:6">
+      <c r="A65">
         <v>206</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B65" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" t="s">
         <v>8</v>
       </c>
-      <c r="D63" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="13">
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="14">
         <v>45746</v>
       </c>
-      <c r="F63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" customFormat="1" spans="1:6">
-      <c r="A64">
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" spans="1:6">
+      <c r="A66">
         <v>21</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B66" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" t="s">
         <v>8</v>
       </c>
-      <c r="D64" t="s">
-        <v>78</v>
-      </c>
-      <c r="E64" s="13">
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="14">
         <v>45747</v>
       </c>
-      <c r="F64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" customFormat="1" spans="5:5">
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" customFormat="1" spans="2:5">
-      <c r="B66" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E66" s="13"/>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="67" customFormat="1" spans="5:5">
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" customFormat="1" spans="1:6">
-      <c r="A68">
+      <c r="E67" s="14"/>
+    </row>
+    <row r="68" customFormat="1" spans="2:5">
+      <c r="B68" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="14"/>
+    </row>
+    <row r="69" customFormat="1" spans="5:5">
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" customFormat="1" spans="1:6">
+      <c r="A70">
         <v>2</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B70" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" t="s">
         <v>24</v>
       </c>
-      <c r="D68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E68" s="13">
+      <c r="D70" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70" s="14">
         <v>45747</v>
       </c>
-      <c r="F68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" customFormat="1" spans="1:6">
-      <c r="A69">
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" spans="1:6">
+      <c r="A71">
         <v>141</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B71" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" t="s">
         <v>8</v>
       </c>
-      <c r="D69" t="s">
-        <v>82</v>
-      </c>
-      <c r="E69" s="13">
+      <c r="D71" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" s="14">
         <v>45748</v>
       </c>
-      <c r="F69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" ht="35" customHeight="1" spans="2:2">
-      <c r="B71" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73">
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" ht="35" customHeight="1" spans="2:2">
+      <c r="B73" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
         <v>226</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B75" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
         <v>8</v>
       </c>
-      <c r="D73" t="s">
-        <v>85</v>
-      </c>
-      <c r="E73" s="13">
+      <c r="D75" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="14">
         <v>45733</v>
       </c>
-      <c r="F73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" ht="39" customHeight="1" spans="2:2">
-      <c r="B75" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77">
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" ht="39" customHeight="1" spans="2:2">
+      <c r="B77" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
         <v>704</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B79" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
         <v>8</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D79" t="s">
+        <v>92</v>
+      </c>
+      <c r="E79" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <v>33</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" s="14">
+        <v>45759</v>
+      </c>
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" ht="32" customHeight="1" spans="2:2">
+      <c r="B82" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" ht="30" customHeight="1" spans="1:6">
+      <c r="A84">
+        <v>34</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84" t="s">
+        <v>97</v>
+      </c>
+      <c r="E84" s="14">
+        <v>45773</v>
+      </c>
+      <c r="F84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" ht="29" customHeight="1" spans="2:2">
+      <c r="B86" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>226</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E77" s="13">
-        <v>45757</v>
-      </c>
-      <c r="F77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78">
-        <v>33</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>99</v>
+      </c>
+      <c r="E88" s="14">
+        <v>45774</v>
+      </c>
+      <c r="F88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89">
+        <v>104</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>101</v>
+      </c>
+      <c r="E89" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>100</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>104</v>
+      </c>
+      <c r="E93" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>102</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C94" t="s">
         <v>24</v>
       </c>
-      <c r="D78" t="s">
-        <v>90</v>
-      </c>
-      <c r="E78" s="13">
-        <v>45759</v>
-      </c>
-      <c r="F78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" ht="32" customHeight="1" spans="2:2">
-      <c r="B80" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="82" ht="30" customHeight="1" spans="1:6">
-      <c r="A82">
-        <v>34</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="D94" t="s">
+        <v>106</v>
+      </c>
+      <c r="E94" s="14">
+        <v>45785</v>
+      </c>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" ht="27" customHeight="1" spans="2:2">
+      <c r="B96" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>235</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98" t="s">
         <v>24</v>
       </c>
-      <c r="D82" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="13">
-        <v>45773</v>
-      </c>
-      <c r="F82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" ht="29" customHeight="1" spans="2:2">
-      <c r="B84" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86">
-        <v>226</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" t="s">
-        <v>95</v>
-      </c>
-      <c r="E86" s="13">
-        <v>45774</v>
-      </c>
-      <c r="F86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87">
-        <v>104</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C87" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" t="s">
-        <v>97</v>
-      </c>
-      <c r="E87" s="13">
-        <v>45782</v>
-      </c>
-      <c r="F87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2">
-      <c r="B89" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91">
-        <v>100</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" t="s">
-        <v>100</v>
-      </c>
-      <c r="E91" s="13">
-        <v>45784</v>
-      </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92">
-        <v>102</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C92" t="s">
-        <v>24</v>
-      </c>
-      <c r="D92" t="s">
-        <v>102</v>
-      </c>
-      <c r="E92" s="13">
-        <v>45785</v>
-      </c>
-      <c r="F92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" ht="27" customHeight="1" spans="2:2">
-      <c r="B94" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96">
-        <v>235</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C96" t="s">
-        <v>24</v>
-      </c>
-      <c r="D96" t="s">
-        <v>105</v>
-      </c>
-      <c r="E96" s="13">
+      <c r="D98" t="s">
+        <v>109</v>
+      </c>
+      <c r="E98" s="14">
         <v>45786</v>
       </c>
-      <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" ht="24" customHeight="1" spans="2:2">
-      <c r="B98" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100">
-        <v>133</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C100" t="s">
-        <v>24</v>
-      </c>
-      <c r="D100" t="s">
-        <v>108</v>
-      </c>
-      <c r="E100" s="13">
-        <v>45791</v>
-      </c>
-      <c r="F100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101">
-        <v>200</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C101" t="s">
-        <v>24</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="F98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" ht="24" customHeight="1" spans="2:2">
+      <c r="B100" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E101" s="13">
-        <v>45806</v>
-      </c>
-      <c r="F101" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>2359</v>
+        <v>133</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>111</v>
@@ -2802,90 +2824,130 @@
       <c r="D102" t="s">
         <v>112</v>
       </c>
-      <c r="E102" s="13">
+      <c r="E102" s="14">
+        <v>45791</v>
+      </c>
+      <c r="F102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>200</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" t="s">
+        <v>114</v>
+      </c>
+      <c r="E103" s="14">
+        <v>45806</v>
+      </c>
+      <c r="F103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>2359</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" t="s">
+        <v>116</v>
+      </c>
+      <c r="E104" s="14">
         <v>45807</v>
       </c>
-      <c r="F102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" ht="29" customHeight="1" spans="2:2">
-      <c r="B104" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106">
+      <c r="F104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" ht="29" customHeight="1" spans="2:2">
+      <c r="B106" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
         <v>106</v>
       </c>
-      <c r="B106" t="s">
-        <v>114</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="B108" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C108" t="s">
         <v>24</v>
       </c>
-      <c r="D106" t="s">
-        <v>115</v>
-      </c>
-      <c r="E106" s="13">
+      <c r="D108" t="s">
+        <v>119</v>
+      </c>
+      <c r="E108" s="14">
         <v>45782</v>
       </c>
-      <c r="F106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107">
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
         <v>207</v>
       </c>
-      <c r="B107" t="s">
-        <v>116</v>
-      </c>
-      <c r="C107" t="s">
+      <c r="B109" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109" t="s">
         <v>24</v>
       </c>
-      <c r="D107" t="s">
-        <v>117</v>
-      </c>
-      <c r="E107" s="13">
+      <c r="D109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" s="14">
         <v>45817</v>
       </c>
-      <c r="F107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" ht="41" customHeight="1" spans="1:2">
-      <c r="A117" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B117" s="16">
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" ht="41" customHeight="1" spans="1:2">
+      <c r="A119" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B119" s="17">
         <f>COUNT(A:A)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="119" ht="30" customHeight="1" spans="1:2">
-      <c r="A119" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B119" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" ht="30" customHeight="1" spans="1:2">
+      <c r="A121" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121" s="19">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>19</v>
       </c>
     </row>
-    <row r="120" ht="40" customHeight="1" spans="1:2">
-      <c r="A120" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B120" s="20">
+    <row r="122" ht="40" customHeight="1" spans="1:2">
+      <c r="A122" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" s="21">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="121" ht="36" customHeight="1" spans="1:2">
-      <c r="A121" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B121" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" ht="36" customHeight="1" spans="1:2">
+      <c r="A123" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" s="23">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
2200. Find All K-Distant Indices in an Array( Two pointers )
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
   <si>
     <t>Q No.</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>DFS , Topological Sort ,Cycle detection</t>
+  </si>
+  <si>
+    <t>Graphs (hard)</t>
+  </si>
+  <si>
+    <t>127. Word Ladder</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>BFS,Adjacency List , Hashtable</t>
   </si>
   <si>
     <t>Total Question Solved:</t>
@@ -418,7 +430,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +506,13 @@
       <i/>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0A84FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1023,137 +1042,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1200,6 +1219,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1768,8 +1790,8 @@
   <sheetPr/>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2916,43 +2938,71 @@
         <v>10</v>
       </c>
     </row>
+    <row r="111" ht="35" customHeight="1" spans="2:2">
+      <c r="B111" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>127</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113" t="s">
+        <v>124</v>
+      </c>
+      <c r="D113" t="s">
+        <v>125</v>
+      </c>
+      <c r="E113" s="14">
+        <v>45831</v>
+      </c>
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="119" ht="41" customHeight="1" spans="1:2">
-      <c r="A119" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B119" s="17">
+      <c r="A119" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B119" s="18">
         <f>COUNT(A:A)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" ht="30" customHeight="1" spans="1:2">
-      <c r="A121" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B121" s="19">
+      <c r="A121" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B121" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>19</v>
       </c>
     </row>
     <row r="122" ht="40" customHeight="1" spans="1:2">
-      <c r="A122" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B122" s="21">
+      <c r="A122" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B122" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>30</v>
       </c>
     </row>
     <row r="123" ht="36" customHeight="1" spans="1:2">
-      <c r="A123" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B123" s="23">
+      <c r="A123" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B123" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B113" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
733. Flood Fill (BFS)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="132">
   <si>
     <t>Q No.</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>Directed graph,DFS ,Hashmap , distance calculation</t>
+  </si>
+  <si>
+    <t>Flood Fill</t>
+  </si>
+  <si>
+    <t>BFS</t>
   </si>
   <si>
     <t>Graphs (advanced)</t>
@@ -1788,10 +1794,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2893,34 +2899,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" ht="29" customHeight="1" spans="2:2">
-      <c r="B106" s="4" t="s">
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>733</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108">
-        <v>106</v>
-      </c>
-      <c r="B108" s="5" t="s">
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
         <v>118</v>
       </c>
-      <c r="C108" t="s">
-        <v>24</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="E105" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" ht="29" customHeight="1" spans="2:2">
+      <c r="B107" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="E108" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F108" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>120</v>
@@ -2932,76 +2938,96 @@
         <v>121</v>
       </c>
       <c r="E109" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
+        <v>207</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C110" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" t="s">
+        <v>123</v>
+      </c>
+      <c r="E110" s="14">
         <v>45817</v>
       </c>
-      <c r="F109" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111" ht="35" customHeight="1" spans="2:2">
-      <c r="B111" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113">
+      <c r="F110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" ht="35" customHeight="1" spans="2:2">
+      <c r="B112" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
         <v>127</v>
       </c>
-      <c r="B113" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C113" t="s">
-        <v>124</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="B114" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E113" s="14">
+      <c r="C114" t="s">
+        <v>126</v>
+      </c>
+      <c r="D114" t="s">
+        <v>127</v>
+      </c>
+      <c r="E114" s="14">
         <v>45831</v>
       </c>
-      <c r="F113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" ht="41" customHeight="1" spans="1:2">
-      <c r="A119" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" s="18">
+      <c r="F114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" ht="41" customHeight="1" spans="1:2">
+      <c r="A120" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120" s="18">
         <f>COUNT(A:A)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="121" ht="30" customHeight="1" spans="1:2">
-      <c r="A121" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B121" s="20">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="122" ht="30" customHeight="1" spans="1:2">
+      <c r="A122" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B122" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="122" ht="40" customHeight="1" spans="1:2">
-      <c r="A122" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B122" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" ht="40" customHeight="1" spans="1:2">
+      <c r="A123" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B123" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>30</v>
       </c>
     </row>
-    <row r="123" ht="36" customHeight="1" spans="1:2">
-      <c r="A123" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B123" s="24">
+    <row r="124" ht="36" customHeight="1" spans="1:2">
+      <c r="A124" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B124" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B113" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B114" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
994. Rotting Oranges ( Multi Source BFS )
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15960"/>
+    <workbookView windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="134">
   <si>
     <t>Q No.</t>
   </si>
@@ -302,7 +302,7 @@
     <t>Binary Search (basic)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Binary Search</t>
+    <t>Binary Search</t>
   </si>
   <si>
     <t>Binary Search , recursion</t>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>BFS</t>
+  </si>
+  <si>
+    <t>Rotting Oranges</t>
+  </si>
+  <si>
+    <t>Multi-Source BFS , Deque</t>
   </si>
   <si>
     <t>Graphs (advanced)</t>
@@ -1794,10 +1800,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1825,7 +1831,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2919,34 +2925,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" ht="29" customHeight="1" spans="2:2">
-      <c r="B107" s="4" t="s">
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>994</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109">
-        <v>106</v>
-      </c>
-      <c r="B109" s="5" t="s">
+      <c r="C106" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" t="s">
         <v>120</v>
       </c>
-      <c r="C109" t="s">
-        <v>24</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="E106" s="14">
+        <v>45834</v>
+      </c>
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" ht="29" customHeight="1" spans="2:2">
+      <c r="B108" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="E109" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F109" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>122</v>
@@ -2958,76 +2964,96 @@
         <v>123</v>
       </c>
       <c r="E110" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
+        <v>207</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C111" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" t="s">
+        <v>125</v>
+      </c>
+      <c r="E111" s="14">
         <v>45817</v>
       </c>
-      <c r="F110" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" ht="35" customHeight="1" spans="2:2">
-      <c r="B112" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114">
+      <c r="F111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" ht="35" customHeight="1" spans="2:2">
+      <c r="B113" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115">
         <v>127</v>
       </c>
-      <c r="B114" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C114" t="s">
-        <v>126</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="B115" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E114" s="14">
+      <c r="C115" t="s">
+        <v>128</v>
+      </c>
+      <c r="D115" t="s">
+        <v>129</v>
+      </c>
+      <c r="E115" s="14">
         <v>45831</v>
       </c>
-      <c r="F114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" ht="41" customHeight="1" spans="1:2">
-      <c r="A120" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B120" s="18">
+      <c r="F115" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" ht="41" customHeight="1" spans="1:2">
+      <c r="A121" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B121" s="18">
         <f>COUNT(A:A)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="122" ht="30" customHeight="1" spans="1:2">
-      <c r="A122" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B122" s="20">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="123" ht="30" customHeight="1" spans="1:2">
+      <c r="A123" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B123" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>20</v>
       </c>
     </row>
-    <row r="123" ht="40" customHeight="1" spans="1:2">
-      <c r="A123" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B123" s="22">
+    <row r="124" ht="40" customHeight="1" spans="1:2">
+      <c r="A124" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="124" ht="36" customHeight="1" spans="1:2">
-      <c r="A124" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B124" s="24">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="125" ht="36" customHeight="1" spans="1:2">
+      <c r="A125" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B125" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B114" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B115" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2099. Find Subsequence of Length K With the Largest Sum  (Priority Queue)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="136">
   <si>
     <t>Q No.</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t>Array,Min Heap</t>
+  </si>
+  <si>
+    <t>Find Subsequence of Length K With the Largest Sum</t>
+  </si>
+  <si>
+    <t>Array , Hashmap , Priority Queue/heap</t>
   </si>
   <si>
     <t>Stack (Basics)</t>
@@ -1800,10 +1806,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2443,126 +2449,126 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" ht="38" customHeight="1" spans="2:2">
-      <c r="B52" s="11" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>2099</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>20</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
         <v>69</v>
       </c>
-      <c r="C54" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E51" s="14">
+        <v>45836</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" ht="38" customHeight="1" spans="2:2">
+      <c r="B53" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="E54" s="14">
-        <v>45719</v>
-      </c>
-      <c r="F54" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
         <v>72</v>
       </c>
       <c r="E55" s="14">
+        <v>45719</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>155</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56" s="14">
         <v>45731</v>
       </c>
-      <c r="F55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" ht="40" customHeight="1" spans="2:2">
-      <c r="B57" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" ht="40" customHeight="1" spans="2:2">
+      <c r="B58" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
         <v>739</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B60" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" t="s">
         <v>24</v>
       </c>
-      <c r="D59" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="14">
+      <c r="D60" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" s="14">
         <v>45732</v>
       </c>
-      <c r="F59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" s="1" customFormat="1" spans="1:6">
-      <c r="A60" s="1">
+      <c r="F60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" s="1" customFormat="1" spans="1:6">
+      <c r="A61" s="1">
         <v>84</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="B61" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" s="15">
+      <c r="E61" s="15">
         <v>45745</v>
       </c>
-      <c r="F60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B63" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" customFormat="1" ht="18" spans="1:6">
-      <c r="A65">
+      <c r="F61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B64" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" customFormat="1" ht="18" spans="1:6">
+      <c r="A66">
         <v>206</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C65" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" t="s">
-        <v>80</v>
-      </c>
-      <c r="E65" s="14">
-        <v>45746</v>
-      </c>
-      <c r="F65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" customFormat="1" spans="1:6">
-      <c r="A66">
-        <v>21</v>
-      </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C66" t="s">
@@ -2572,190 +2578,190 @@
         <v>82</v>
       </c>
       <c r="E66" s="14">
+        <v>45746</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" spans="1:6">
+      <c r="A67">
+        <v>21</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="14">
         <v>45747</v>
       </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" customFormat="1" spans="5:5">
-      <c r="E67" s="14"/>
-    </row>
-    <row r="68" customFormat="1" spans="2:5">
-      <c r="B68" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" spans="5:5">
       <c r="E68" s="14"/>
     </row>
-    <row r="69" customFormat="1" spans="5:5">
+    <row r="69" customFormat="1" spans="2:5">
+      <c r="B69" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="E69" s="14"/>
     </row>
-    <row r="70" customFormat="1" spans="1:6">
-      <c r="A70">
-        <v>2</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C70" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70" t="s">
-        <v>82</v>
-      </c>
-      <c r="E70" s="14">
-        <v>45747</v>
-      </c>
-      <c r="F70" t="s">
-        <v>10</v>
-      </c>
+    <row r="70" customFormat="1" spans="5:5">
+      <c r="E70" s="14"/>
     </row>
     <row r="71" customFormat="1" spans="1:6">
       <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" spans="1:6">
+      <c r="A72">
         <v>141</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B72" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
         <v>8</v>
       </c>
-      <c r="D71" t="s">
-        <v>86</v>
-      </c>
-      <c r="E71" s="14">
+      <c r="D72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" s="14">
         <v>45748</v>
       </c>
-      <c r="F71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" ht="35" customHeight="1" spans="2:2">
-      <c r="B73" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75">
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" ht="35" customHeight="1" spans="2:2">
+      <c r="B74" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
         <v>226</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="B76" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" t="s">
         <v>8</v>
       </c>
-      <c r="D75" t="s">
-        <v>89</v>
-      </c>
-      <c r="E75" s="14">
+      <c r="D76" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="14">
         <v>45733</v>
       </c>
-      <c r="F75" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" ht="39" customHeight="1" spans="2:2">
-      <c r="B77" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79">
-        <v>704</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" ht="39" customHeight="1" spans="2:2">
+      <c r="B78" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="E79" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F79" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C80" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D80" t="s">
         <v>94</v>
       </c>
       <c r="E80" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <v>33</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="14">
         <v>45759</v>
       </c>
-      <c r="F80" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" ht="32" customHeight="1" spans="2:2">
-      <c r="B82" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="84" ht="30" customHeight="1" spans="1:6">
-      <c r="A84">
+      <c r="F81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" ht="32" customHeight="1" spans="2:2">
+      <c r="B83" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" ht="30" customHeight="1" spans="1:6">
+      <c r="A85">
         <v>34</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B85" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" t="s">
         <v>24</v>
       </c>
-      <c r="D84" t="s">
-        <v>97</v>
-      </c>
-      <c r="E84" s="14">
+      <c r="D85" t="s">
+        <v>99</v>
+      </c>
+      <c r="E85" s="14">
         <v>45773</v>
       </c>
-      <c r="F84" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" ht="29" customHeight="1" spans="2:2">
-      <c r="B86" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88">
-        <v>226</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" t="s">
-        <v>99</v>
-      </c>
-      <c r="E88" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F88" t="s">
-        <v>10</v>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" ht="29" customHeight="1" spans="2:2">
+      <c r="B87" s="11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
@@ -2764,110 +2770,110 @@
         <v>101</v>
       </c>
       <c r="E89" s="14">
+        <v>45774</v>
+      </c>
+      <c r="F89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <v>104</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="14">
         <v>45782</v>
       </c>
-      <c r="F89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93">
-        <v>100</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C93" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="F90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="E93" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F93" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C94" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D94" t="s">
         <v>106</v>
       </c>
       <c r="E94" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>102</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C95" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" t="s">
+        <v>108</v>
+      </c>
+      <c r="E95" s="14">
         <v>45785</v>
       </c>
-      <c r="F94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" ht="27" customHeight="1" spans="2:2">
-      <c r="B96" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98">
+      <c r="F95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" ht="27" customHeight="1" spans="2:2">
+      <c r="B97" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
         <v>235</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" t="s">
         <v>24</v>
       </c>
-      <c r="D98" t="s">
-        <v>109</v>
-      </c>
-      <c r="E98" s="14">
+      <c r="D99" t="s">
+        <v>111</v>
+      </c>
+      <c r="E99" s="14">
         <v>45786</v>
       </c>
-      <c r="F98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100" ht="24" customHeight="1" spans="2:2">
-      <c r="B100" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102">
-        <v>133</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C102" t="s">
-        <v>24</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" ht="24" customHeight="1" spans="2:2">
+      <c r="B101" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="E102" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F102" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>113</v>
@@ -2879,7 +2885,7 @@
         <v>114</v>
       </c>
       <c r="E103" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F103" t="s">
         <v>10</v>
@@ -2887,7 +2893,7 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>115</v>
@@ -2899,7 +2905,7 @@
         <v>116</v>
       </c>
       <c r="E104" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -2907,19 +2913,19 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D105" t="s">
         <v>118</v>
       </c>
       <c r="E105" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -2927,52 +2933,52 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D106" t="s">
         <v>120</v>
       </c>
       <c r="E106" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>994</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C107" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" t="s">
+        <v>122</v>
+      </c>
+      <c r="E107" s="14">
         <v>45834</v>
       </c>
-      <c r="F106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" ht="29" customHeight="1" spans="2:2">
-      <c r="B108" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110">
-        <v>106</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C110" t="s">
-        <v>24</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" ht="29" customHeight="1" spans="2:2">
+      <c r="B109" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E110" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F110" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>124</v>
@@ -2984,76 +2990,96 @@
         <v>125</v>
       </c>
       <c r="E111" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
+        <v>207</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" s="14">
         <v>45817</v>
       </c>
-      <c r="F111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" ht="35" customHeight="1" spans="2:2">
-      <c r="B113" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115">
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" ht="35" customHeight="1" spans="2:2">
+      <c r="B114" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
         <v>127</v>
       </c>
-      <c r="B115" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C115" t="s">
-        <v>128</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="B116" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E115" s="14">
+      <c r="C116" t="s">
+        <v>130</v>
+      </c>
+      <c r="D116" t="s">
+        <v>131</v>
+      </c>
+      <c r="E116" s="14">
         <v>45831</v>
       </c>
-      <c r="F115" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" ht="41" customHeight="1" spans="1:2">
-      <c r="A121" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B121" s="18">
+      <c r="F116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" ht="41" customHeight="1" spans="1:2">
+      <c r="A122" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B122" s="18">
         <f>COUNT(A:A)</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="123" ht="30" customHeight="1" spans="1:2">
-      <c r="A123" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B123" s="20">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="124" ht="30" customHeight="1" spans="1:2">
+      <c r="A124" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" ht="40" customHeight="1" spans="1:2">
-      <c r="A124" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B124" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125" ht="40" customHeight="1" spans="1:2">
+      <c r="A125" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B125" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>31</v>
       </c>
     </row>
-    <row r="125" ht="36" customHeight="1" spans="1:2">
-      <c r="A125" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B125" s="24">
+    <row r="126" ht="36" customHeight="1" spans="1:2">
+      <c r="A126" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B126" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B115" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B116" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
594. Longest Harmonious Subsequence (Sliding window)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="138">
   <si>
     <t>Q No.</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Array , Sliding Window</t>
+  </si>
+  <si>
+    <t>Longest Harmonious Subsequence</t>
+  </si>
+  <si>
+    <t>Array , Counting,Hashtable,Sliding Window ,Sorting</t>
   </si>
   <si>
     <t>Sliding Window (Advance)</t>
@@ -1806,10 +1812,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2355,40 +2361,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="9"/>
-      <c r="E41" s="14"/>
-    </row>
-    <row r="42" ht="39" customHeight="1" spans="2:2">
-      <c r="B42" s="4" t="s">
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>594</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" ht="17" spans="1:6">
-      <c r="A44">
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="14">
+        <v>45838</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="9"/>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" ht="39" customHeight="1" spans="2:2">
+      <c r="B43" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" ht="17" spans="1:6">
+      <c r="A45">
         <v>424</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="14">
-        <v>45716</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
-        <v>2799</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C45" t="s">
@@ -2398,7 +2404,7 @@
         <v>62</v>
       </c>
       <c r="E45" s="14">
-        <v>45771</v>
+        <v>45716</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
@@ -2406,7 +2412,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>2962</v>
+        <v>2799</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>63</v>
@@ -2418,177 +2424,177 @@
         <v>64</v>
       </c>
       <c r="E46" s="14">
+        <v>45771</v>
+      </c>
+      <c r="F46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>2962</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="14">
         <v>45776</v>
       </c>
-      <c r="F46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" ht="31" customHeight="1" spans="2:2">
-      <c r="B48" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50">
-        <v>3066</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="F47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" ht="31" customHeight="1" spans="2:2">
+      <c r="B49" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="E50" s="14">
-        <v>45701</v>
-      </c>
-      <c r="F50" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>2099</v>
+        <v>3066</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
         <v>69</v>
       </c>
       <c r="E51" s="14">
+        <v>45701</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>2099</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="14">
         <v>45836</v>
       </c>
-      <c r="F51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" ht="38" customHeight="1" spans="2:2">
-      <c r="B53" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>20</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" ht="38" customHeight="1" spans="2:2">
+      <c r="B54" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="E55" s="14">
-        <v>45719</v>
-      </c>
-      <c r="F55" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
         <v>74</v>
       </c>
       <c r="E56" s="14">
+        <v>45719</v>
+      </c>
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>155</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="14">
         <v>45731</v>
       </c>
-      <c r="F56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" ht="40" customHeight="1" spans="2:2">
-      <c r="B58" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60">
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" ht="40" customHeight="1" spans="2:2">
+      <c r="B59" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
         <v>739</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B61" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" t="s">
         <v>24</v>
       </c>
-      <c r="D60" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="14">
+      <c r="D61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="14">
         <v>45732</v>
       </c>
-      <c r="F60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" s="1" customFormat="1" spans="1:6">
-      <c r="A61" s="1">
+      <c r="F61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:6">
+      <c r="A62" s="1">
         <v>84</v>
       </c>
-      <c r="B61" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="B62" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" s="15">
+      <c r="E62" s="15">
         <v>45745</v>
       </c>
-      <c r="F61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B64" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" customFormat="1" ht="18" spans="1:6">
-      <c r="A66">
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B65" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" customFormat="1" ht="18" spans="1:6">
+      <c r="A67">
         <v>206</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" t="s">
-        <v>82</v>
-      </c>
-      <c r="E66" s="14">
-        <v>45746</v>
-      </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" customFormat="1" spans="1:6">
-      <c r="A67">
-        <v>21</v>
-      </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C67" t="s">
@@ -2598,190 +2604,190 @@
         <v>84</v>
       </c>
       <c r="E67" s="14">
+        <v>45746</v>
+      </c>
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" spans="1:6">
+      <c r="A68">
+        <v>21</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68" s="14">
         <v>45747</v>
       </c>
-      <c r="F67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" spans="5:5">
-      <c r="E68" s="14"/>
-    </row>
-    <row r="69" customFormat="1" spans="2:5">
-      <c r="B69" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" customFormat="1" spans="5:5">
       <c r="E69" s="14"/>
     </row>
-    <row r="70" customFormat="1" spans="5:5">
+    <row r="70" customFormat="1" spans="2:5">
+      <c r="B70" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="E70" s="14"/>
     </row>
-    <row r="71" customFormat="1" spans="1:6">
-      <c r="A71">
-        <v>2</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C71" t="s">
-        <v>24</v>
-      </c>
-      <c r="D71" t="s">
-        <v>84</v>
-      </c>
-      <c r="E71" s="14">
-        <v>45747</v>
-      </c>
-      <c r="F71" t="s">
-        <v>10</v>
-      </c>
+    <row r="71" customFormat="1" spans="5:5">
+      <c r="E71" s="14"/>
     </row>
     <row r="72" customFormat="1" spans="1:6">
       <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" spans="1:6">
+      <c r="A73">
         <v>141</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B73" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" t="s">
         <v>8</v>
       </c>
-      <c r="D72" t="s">
-        <v>88</v>
-      </c>
-      <c r="E72" s="14">
+      <c r="D73" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="14">
         <v>45748</v>
       </c>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" ht="35" customHeight="1" spans="2:2">
-      <c r="B74" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76">
+      <c r="F73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" ht="35" customHeight="1" spans="2:2">
+      <c r="B75" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
         <v>226</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="B77" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" t="s">
         <v>8</v>
       </c>
-      <c r="D76" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="14">
+      <c r="D77" t="s">
+        <v>93</v>
+      </c>
+      <c r="E77" s="14">
         <v>45733</v>
       </c>
-      <c r="F76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" ht="39" customHeight="1" spans="2:2">
-      <c r="B78" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80">
-        <v>704</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C80" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" ht="39" customHeight="1" spans="2:2">
+      <c r="B79" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="E80" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F80" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C81" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D81" t="s">
         <v>96</v>
       </c>
       <c r="E81" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>33</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" t="s">
+        <v>98</v>
+      </c>
+      <c r="E82" s="14">
         <v>45759</v>
       </c>
-      <c r="F81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" ht="32" customHeight="1" spans="2:2">
-      <c r="B83" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="85" ht="30" customHeight="1" spans="1:6">
-      <c r="A85">
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" ht="32" customHeight="1" spans="2:2">
+      <c r="B84" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" ht="30" customHeight="1" spans="1:6">
+      <c r="A86">
         <v>34</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="B86" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" t="s">
         <v>24</v>
       </c>
-      <c r="D85" t="s">
-        <v>99</v>
-      </c>
-      <c r="E85" s="14">
+      <c r="D86" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="14">
         <v>45773</v>
       </c>
-      <c r="F85" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" ht="29" customHeight="1" spans="2:2">
-      <c r="B87" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89">
-        <v>226</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" t="s">
-        <v>101</v>
-      </c>
-      <c r="E89" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F89" t="s">
-        <v>10</v>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" ht="29" customHeight="1" spans="2:2">
+      <c r="B88" s="11" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C90" t="s">
         <v>8</v>
@@ -2790,110 +2796,110 @@
         <v>103</v>
       </c>
       <c r="E90" s="14">
+        <v>45774</v>
+      </c>
+      <c r="F90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>104</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>105</v>
+      </c>
+      <c r="E91" s="14">
         <v>45782</v>
       </c>
-      <c r="F90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94">
-        <v>100</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="E94" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F94" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D95" t="s">
         <v>108</v>
       </c>
       <c r="E95" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>102</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" t="s">
+        <v>110</v>
+      </c>
+      <c r="E96" s="14">
         <v>45785</v>
       </c>
-      <c r="F95" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" ht="27" customHeight="1" spans="2:2">
-      <c r="B97" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99">
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" ht="27" customHeight="1" spans="2:2">
+      <c r="B98" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
         <v>235</v>
       </c>
-      <c r="B99" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B100" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="s">
         <v>24</v>
       </c>
-      <c r="D99" t="s">
-        <v>111</v>
-      </c>
-      <c r="E99" s="14">
+      <c r="D100" t="s">
+        <v>113</v>
+      </c>
+      <c r="E100" s="14">
         <v>45786</v>
       </c>
-      <c r="F99" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" ht="24" customHeight="1" spans="2:2">
-      <c r="B101" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103">
-        <v>133</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C103" t="s">
-        <v>24</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" ht="24" customHeight="1" spans="2:2">
+      <c r="B102" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="E103" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F103" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>115</v>
@@ -2905,7 +2911,7 @@
         <v>116</v>
       </c>
       <c r="E104" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -2913,7 +2919,7 @@
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>117</v>
@@ -2925,7 +2931,7 @@
         <v>118</v>
       </c>
       <c r="E105" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -2933,19 +2939,19 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C106" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D106" t="s">
         <v>120</v>
       </c>
       <c r="E106" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -2953,52 +2959,52 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C107" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D107" t="s">
         <v>122</v>
       </c>
       <c r="E107" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
+        <v>994</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C108" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" t="s">
+        <v>124</v>
+      </c>
+      <c r="E108" s="14">
         <v>45834</v>
       </c>
-      <c r="F107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" ht="29" customHeight="1" spans="2:2">
-      <c r="B109" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111">
-        <v>106</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C111" t="s">
-        <v>24</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" ht="29" customHeight="1" spans="2:2">
+      <c r="B110" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="E111" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F111" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>126</v>
@@ -3010,76 +3016,96 @@
         <v>127</v>
       </c>
       <c r="E112" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>207</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C113" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" t="s">
+        <v>129</v>
+      </c>
+      <c r="E113" s="14">
         <v>45817</v>
       </c>
-      <c r="F112" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" ht="35" customHeight="1" spans="2:2">
-      <c r="B114" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116">
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" ht="35" customHeight="1" spans="2:2">
+      <c r="B115" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
         <v>127</v>
       </c>
-      <c r="B116" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C116" t="s">
-        <v>130</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="B117" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E116" s="14">
+      <c r="C117" t="s">
+        <v>132</v>
+      </c>
+      <c r="D117" t="s">
+        <v>133</v>
+      </c>
+      <c r="E117" s="14">
         <v>45831</v>
       </c>
-      <c r="F116" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" ht="41" customHeight="1" spans="1:2">
-      <c r="A122" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B122" s="18">
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" ht="41" customHeight="1" spans="1:2">
+      <c r="A123" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B123" s="18">
         <f>COUNT(A:A)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="124" ht="30" customHeight="1" spans="1:2">
-      <c r="A124" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B124" s="20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="125" ht="30" customHeight="1" spans="1:2">
+      <c r="A125" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B125" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="125" ht="40" customHeight="1" spans="1:2">
-      <c r="A125" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="B125" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" ht="40" customHeight="1" spans="1:2">
+      <c r="A126" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B126" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>31</v>
       </c>
     </row>
-    <row r="126" ht="36" customHeight="1" spans="1:2">
-      <c r="A126" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="B126" s="24">
+    <row r="127" ht="36" customHeight="1" spans="1:2">
+      <c r="A127" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B127" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B116" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B117" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
101. Symmetric Tree (DFS -recursion)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
   <si>
     <t>Q No.</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Binary Tree,recurson</t>
+  </si>
+  <si>
+    <t>Symmetric Tree</t>
+  </si>
+  <si>
+    <t>DFS ,recursion</t>
   </si>
   <si>
     <t>Binary Search (basic)</t>
@@ -1812,10 +1818,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2707,107 +2713,107 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" ht="39" customHeight="1" spans="2:2">
-      <c r="B79" s="11" t="s">
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>101</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81">
-        <v>704</v>
-      </c>
-      <c r="B81" s="5" t="s">
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
         <v>95</v>
       </c>
-      <c r="C81" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E78" s="14">
+        <v>45839</v>
+      </c>
+      <c r="F78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" ht="39" customHeight="1" spans="2:2">
+      <c r="B80" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="E81" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F81" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>33</v>
+        <v>704</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C82" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D82" t="s">
         <v>98</v>
       </c>
       <c r="E82" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>33</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C83" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" t="s">
+        <v>100</v>
+      </c>
+      <c r="E83" s="14">
         <v>45759</v>
       </c>
-      <c r="F82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" ht="32" customHeight="1" spans="2:2">
-      <c r="B84" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="86" ht="30" customHeight="1" spans="1:6">
-      <c r="A86">
+      <c r="F83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" ht="32" customHeight="1" spans="2:2">
+      <c r="B85" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" ht="30" customHeight="1" spans="1:6">
+      <c r="A87">
         <v>34</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B87" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87" t="s">
         <v>24</v>
       </c>
-      <c r="D86" t="s">
-        <v>101</v>
-      </c>
-      <c r="E86" s="14">
+      <c r="D87" t="s">
+        <v>103</v>
+      </c>
+      <c r="E87" s="14">
         <v>45773</v>
       </c>
-      <c r="F86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" ht="29" customHeight="1" spans="2:2">
-      <c r="B88" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90">
-        <v>226</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" t="s">
-        <v>103</v>
-      </c>
-      <c r="E90" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F90" t="s">
-        <v>10</v>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" ht="29" customHeight="1" spans="2:2">
+      <c r="B89" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -2816,110 +2822,110 @@
         <v>105</v>
       </c>
       <c r="E91" s="14">
+        <v>45774</v>
+      </c>
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>104</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>107</v>
+      </c>
+      <c r="E92" s="14">
         <v>45782</v>
       </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2">
-      <c r="B93" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95">
-        <v>100</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E95" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F95" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C96" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D96" t="s">
         <v>110</v>
       </c>
       <c r="E96" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>102</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C97" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" t="s">
+        <v>112</v>
+      </c>
+      <c r="E97" s="14">
         <v>45785</v>
       </c>
-      <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" ht="27" customHeight="1" spans="2:2">
-      <c r="B98" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100">
+      <c r="F97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" ht="27" customHeight="1" spans="2:2">
+      <c r="B99" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
         <v>235</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B101" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C101" t="s">
         <v>24</v>
       </c>
-      <c r="D100" t="s">
-        <v>113</v>
-      </c>
-      <c r="E100" s="14">
+      <c r="D101" t="s">
+        <v>115</v>
+      </c>
+      <c r="E101" s="14">
         <v>45786</v>
       </c>
-      <c r="F100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" ht="24" customHeight="1" spans="2:2">
-      <c r="B102" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104">
-        <v>133</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C104" t="s">
-        <v>24</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" ht="24" customHeight="1" spans="2:2">
+      <c r="B103" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="E104" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F104" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>117</v>
@@ -2931,7 +2937,7 @@
         <v>118</v>
       </c>
       <c r="E105" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -2939,7 +2945,7 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>119</v>
@@ -2951,7 +2957,7 @@
         <v>120</v>
       </c>
       <c r="E106" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -2959,19 +2965,19 @@
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>121</v>
       </c>
       <c r="C107" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D107" t="s">
         <v>122</v>
       </c>
       <c r="E107" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F107" t="s">
         <v>10</v>
@@ -2979,52 +2985,52 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D108" t="s">
         <v>124</v>
       </c>
       <c r="E108" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
+        <v>994</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C109" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" t="s">
+        <v>126</v>
+      </c>
+      <c r="E109" s="14">
         <v>45834</v>
       </c>
-      <c r="F108" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" ht="29" customHeight="1" spans="2:2">
-      <c r="B110" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112">
-        <v>106</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" ht="29" customHeight="1" spans="2:2">
+      <c r="B111" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="E112" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F112" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>128</v>
@@ -3036,76 +3042,96 @@
         <v>129</v>
       </c>
       <c r="E113" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
+        <v>207</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C114" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" t="s">
+        <v>131</v>
+      </c>
+      <c r="E114" s="14">
         <v>45817</v>
       </c>
-      <c r="F113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" ht="35" customHeight="1" spans="2:2">
-      <c r="B115" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117">
+      <c r="F114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" ht="35" customHeight="1" spans="2:2">
+      <c r="B116" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
         <v>127</v>
       </c>
-      <c r="B117" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C117" t="s">
-        <v>132</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="B118" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E117" s="14">
+      <c r="C118" t="s">
+        <v>134</v>
+      </c>
+      <c r="D118" t="s">
+        <v>135</v>
+      </c>
+      <c r="E118" s="14">
         <v>45831</v>
       </c>
-      <c r="F117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="123" ht="41" customHeight="1" spans="1:2">
-      <c r="A123" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B123" s="18">
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" ht="41" customHeight="1" spans="1:2">
+      <c r="A124" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B124" s="18">
         <f>COUNT(A:A)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="125" ht="30" customHeight="1" spans="1:2">
-      <c r="A125" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B125" s="20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="126" ht="30" customHeight="1" spans="1:2">
+      <c r="A126" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B126" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="126" ht="40" customHeight="1" spans="1:2">
-      <c r="A126" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B126" s="22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" ht="40" customHeight="1" spans="1:2">
+      <c r="A127" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B127" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>31</v>
       </c>
     </row>
-    <row r="127" ht="36" customHeight="1" spans="1:2">
-      <c r="A127" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="B127" s="24">
+    <row r="128" ht="36" customHeight="1" spans="1:2">
+      <c r="A128" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B117" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B118" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Binary Trees input(using arrays and  Inorder postorder , preorder Traversal
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13680"/>
+    <workbookView windowHeight="13660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
   <si>
     <t>Q No.</t>
   </si>
@@ -275,6 +275,15 @@
     <t>Hard</t>
   </si>
   <si>
+    <t>Queue (Basics)</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queues</t>
+  </si>
+  <si>
+    <t>Deque,stack</t>
+  </si>
+  <si>
     <t>Linked List (Basics)</t>
   </si>
   <si>
@@ -287,7 +296,7 @@
     <t>Merge Two Sorted Lists</t>
   </si>
   <si>
-    <t xml:space="preserve">Linked List </t>
+    <t>Linked List</t>
   </si>
   <si>
     <t>Linked List (Advanced)</t>
@@ -460,7 +469,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,14 +537,6 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1072,137 +1073,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1239,19 +1240,22 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1818,10 +1822,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2572,16 +2576,16 @@
       </c>
     </row>
     <row r="62" s="1" customFormat="1" spans="1:6">
-      <c r="A62" s="1">
+      <c r="A62" s="12">
         <v>84</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E62" s="15">
@@ -2591,413 +2595,378 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B65" s="4" t="s">
+    <row r="64" ht="34" customHeight="1" spans="2:2">
+      <c r="B64" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="67" customFormat="1" ht="18" spans="1:6">
-      <c r="A67">
+    <row r="66" ht="18" spans="1:6">
+      <c r="A66">
+        <v>225</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66" s="14">
+        <v>45841</v>
+      </c>
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B68" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" customFormat="1" ht="18" spans="1:6">
+      <c r="A70">
         <v>206</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B70" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" t="s">
         <v>8</v>
       </c>
-      <c r="D67" t="s">
-        <v>84</v>
-      </c>
-      <c r="E67" s="14">
+      <c r="D70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="14">
         <v>45746</v>
       </c>
-      <c r="F67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" spans="1:6">
-      <c r="A68">
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" spans="1:6">
+      <c r="A71">
         <v>21</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B71" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
         <v>8</v>
       </c>
-      <c r="D68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="14">
+      <c r="D71" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="14">
         <v>45747</v>
       </c>
-      <c r="F68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" customFormat="1" spans="5:5">
-      <c r="E69" s="14"/>
-    </row>
-    <row r="70" customFormat="1" spans="2:5">
-      <c r="B70" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E70" s="14"/>
-    </row>
-    <row r="71" customFormat="1" spans="5:5">
-      <c r="E71" s="14"/>
-    </row>
-    <row r="72" customFormat="1" spans="1:6">
-      <c r="A72">
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" spans="5:5">
+      <c r="E72" s="14"/>
+    </row>
+    <row r="73" customFormat="1" ht="26" customHeight="1" spans="2:5">
+      <c r="B73" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E73" s="14"/>
+    </row>
+    <row r="74" customFormat="1" spans="5:5">
+      <c r="E74" s="14"/>
+    </row>
+    <row r="75" customFormat="1" spans="1:6">
+      <c r="A75">
         <v>2</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B75" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" t="s">
         <v>24</v>
       </c>
-      <c r="D72" t="s">
-        <v>86</v>
-      </c>
-      <c r="E72" s="14">
+      <c r="D75" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="14">
         <v>45747</v>
       </c>
-      <c r="F72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" spans="1:6">
-      <c r="A73">
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="1" spans="1:6">
+      <c r="A76">
         <v>141</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B76" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C76" t="s">
         <v>8</v>
       </c>
-      <c r="D73" t="s">
-        <v>90</v>
-      </c>
-      <c r="E73" s="14">
+      <c r="D76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E76" s="14">
         <v>45748</v>
       </c>
-      <c r="F73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" ht="35" customHeight="1" spans="2:2">
-      <c r="B75" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77">
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" ht="35" customHeight="1" spans="2:2">
+      <c r="B78" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
         <v>226</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B80" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80" t="s">
         <v>8</v>
       </c>
-      <c r="D77" t="s">
-        <v>93</v>
-      </c>
-      <c r="E77" s="14">
+      <c r="D80" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="14">
         <v>45733</v>
       </c>
-      <c r="F77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78">
+      <c r="F80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
         <v>101</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B81" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C81" t="s">
         <v>8</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D81" t="s">
+        <v>98</v>
+      </c>
+      <c r="E81" s="14">
+        <v>45839</v>
+      </c>
+      <c r="F81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" ht="39" customHeight="1" spans="2:2">
+      <c r="B83" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <v>704</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>33</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" t="s">
+        <v>24</v>
+      </c>
+      <c r="D86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" s="14">
+        <v>45759</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" ht="32" customHeight="1" spans="2:2">
+      <c r="B88" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" ht="30" customHeight="1" spans="1:6">
+      <c r="A90">
+        <v>34</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" t="s">
+        <v>106</v>
+      </c>
+      <c r="E90" s="14">
+        <v>45773</v>
+      </c>
+      <c r="F90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" ht="29" customHeight="1" spans="2:2">
+      <c r="B92" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>226</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E78" s="14">
-        <v>45839</v>
-      </c>
-      <c r="F78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" ht="39" customHeight="1" spans="2:2">
-      <c r="B80" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82">
-        <v>704</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="C94" t="s">
         <v>8</v>
       </c>
-      <c r="D82" t="s">
-        <v>98</v>
-      </c>
-      <c r="E82" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83">
-        <v>33</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="D94" t="s">
+        <v>108</v>
+      </c>
+      <c r="E94" s="14">
+        <v>45774</v>
+      </c>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>104</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>110</v>
+      </c>
+      <c r="E95" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>100</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>102</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C100" t="s">
         <v>24</v>
       </c>
-      <c r="D83" t="s">
-        <v>100</v>
-      </c>
-      <c r="E83" s="14">
-        <v>45759</v>
-      </c>
-      <c r="F83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" ht="32" customHeight="1" spans="2:2">
-      <c r="B85" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="87" ht="30" customHeight="1" spans="1:6">
-      <c r="A87">
-        <v>34</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="D100" t="s">
+        <v>115</v>
+      </c>
+      <c r="E100" s="14">
+        <v>45785</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" ht="27" customHeight="1" spans="2:2">
+      <c r="B102" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>235</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C104" t="s">
         <v>24</v>
       </c>
-      <c r="D87" t="s">
-        <v>103</v>
-      </c>
-      <c r="E87" s="14">
-        <v>45773</v>
-      </c>
-      <c r="F87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" ht="29" customHeight="1" spans="2:2">
-      <c r="B89" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91">
-        <v>226</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" t="s">
-        <v>105</v>
-      </c>
-      <c r="E91" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92">
-        <v>104</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C92" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" t="s">
-        <v>107</v>
-      </c>
-      <c r="E92" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2">
-      <c r="B94" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96">
-        <v>100</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" t="s">
-        <v>110</v>
-      </c>
-      <c r="E96" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97">
-        <v>102</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C97" t="s">
-        <v>24</v>
-      </c>
-      <c r="D97" t="s">
-        <v>112</v>
-      </c>
-      <c r="E97" s="14">
-        <v>45785</v>
-      </c>
-      <c r="F97" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" ht="27" customHeight="1" spans="2:2">
-      <c r="B99" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101">
-        <v>235</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C101" t="s">
-        <v>24</v>
-      </c>
-      <c r="D101" t="s">
-        <v>115</v>
-      </c>
-      <c r="E101" s="14">
+      <c r="D104" t="s">
+        <v>118</v>
+      </c>
+      <c r="E104" s="14">
         <v>45786</v>
       </c>
-      <c r="F101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" ht="24" customHeight="1" spans="2:2">
-      <c r="B103" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105">
-        <v>133</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C105" t="s">
-        <v>24</v>
-      </c>
-      <c r="D105" t="s">
-        <v>118</v>
-      </c>
-      <c r="E105" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106">
-        <v>200</v>
-      </c>
-      <c r="B106" s="5" t="s">
+      <c r="F104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" ht="24" customHeight="1" spans="2:2">
+      <c r="B106" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C106" t="s">
-        <v>24</v>
-      </c>
-      <c r="D106" t="s">
-        <v>120</v>
-      </c>
-      <c r="E106" s="14">
-        <v>45806</v>
-      </c>
-      <c r="F106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107">
-        <v>2359</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C107" t="s">
-        <v>24</v>
-      </c>
-      <c r="D107" t="s">
-        <v>122</v>
-      </c>
-      <c r="E107" s="14">
-        <v>45807</v>
-      </c>
-      <c r="F107" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>733</v>
+        <v>133</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C108" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D108" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E108" s="14">
-        <v>45833</v>
+        <v>45791</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -3005,133 +2974,193 @@
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>994</v>
+        <v>200</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C109" t="s">
         <v>24</v>
       </c>
       <c r="D109" t="s">
+        <v>123</v>
+      </c>
+      <c r="E109" s="14">
+        <v>45806</v>
+      </c>
+      <c r="F109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
+        <v>2359</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" t="s">
+        <v>125</v>
+      </c>
+      <c r="E110" s="14">
+        <v>45807</v>
+      </c>
+      <c r="F110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
+        <v>733</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E109" s="14">
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>127</v>
+      </c>
+      <c r="E111" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
+        <v>994</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
+        <v>129</v>
+      </c>
+      <c r="E112" s="14">
         <v>45834</v>
       </c>
-      <c r="F109" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111" ht="29" customHeight="1" spans="2:2">
-      <c r="B111" s="4" t="s">
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" ht="29" customHeight="1" spans="2:2">
+      <c r="B114" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>106</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C116" t="s">
+        <v>24</v>
+      </c>
+      <c r="D116" t="s">
+        <v>132</v>
+      </c>
+      <c r="E116" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
+        <v>207</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117" t="s">
+        <v>24</v>
+      </c>
+      <c r="D117" t="s">
+        <v>134</v>
+      </c>
+      <c r="E117" s="14">
+        <v>45817</v>
+      </c>
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" ht="35" customHeight="1" spans="2:2">
+      <c r="B119" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
         <v>127</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113">
-        <v>106</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="B121" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C121" t="s">
+        <v>137</v>
+      </c>
+      <c r="D121" t="s">
+        <v>138</v>
+      </c>
+      <c r="E121" s="14">
+        <v>45831</v>
+      </c>
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" ht="41" customHeight="1" spans="1:2">
+      <c r="A127" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" s="19">
+        <f>COUNT(A:A)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" ht="30" customHeight="1" spans="1:2">
+      <c r="A129" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B129" s="21">
+        <f>COUNTIF(C:C,"Easy")</f>
         <v>24</v>
       </c>
-      <c r="D113" t="s">
-        <v>129</v>
-      </c>
-      <c r="E113" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114">
-        <v>207</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C114" t="s">
-        <v>24</v>
-      </c>
-      <c r="D114" t="s">
-        <v>131</v>
-      </c>
-      <c r="E114" s="14">
-        <v>45817</v>
-      </c>
-      <c r="F114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" ht="35" customHeight="1" spans="2:2">
-      <c r="B116" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118">
-        <v>127</v>
-      </c>
-      <c r="B118" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C118" t="s">
-        <v>134</v>
-      </c>
-      <c r="D118" t="s">
-        <v>135</v>
-      </c>
-      <c r="E118" s="14">
-        <v>45831</v>
-      </c>
-      <c r="F118" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="124" ht="41" customHeight="1" spans="1:2">
-      <c r="A124" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B124" s="18">
-        <f>COUNT(A:A)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="126" ht="30" customHeight="1" spans="1:2">
-      <c r="A126" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B126" s="20">
-        <f>COUNTIF(C:C,"Easy")</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="127" ht="40" customHeight="1" spans="1:2">
-      <c r="A127" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B127" s="22">
+    </row>
+    <row r="130" ht="40" customHeight="1" spans="1:2">
+      <c r="A130" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="23">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>31</v>
       </c>
     </row>
-    <row r="128" ht="36" customHeight="1" spans="1:2">
-      <c r="A128" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B128" s="24">
+    <row r="131" ht="36" customHeight="1" spans="1:2">
+      <c r="A131" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B131" s="25">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B118" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B121" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
112. Path Sum (Trees-DFS)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13660"/>
+    <workbookView windowHeight="15960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
   <si>
     <t>Q No.</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>BFS ,DFS  recursion</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>DFS ,recusrion</t>
   </si>
   <si>
     <t>Trees ( Advance )</t>
@@ -1203,7 +1209,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1251,9 +1257,6 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1822,10 +1825,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2604,7 +2607,7 @@
       <c r="A66">
         <v>225</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C66" t="s">
@@ -2877,104 +2880,104 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="2:2">
-      <c r="B97" s="11" t="s">
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>112</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99">
-        <v>100</v>
-      </c>
-      <c r="B99" s="5" t="s">
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
         <v>112</v>
       </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E96" s="14">
+        <v>45842</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="E99" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F99" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C100" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D100" t="s">
         <v>115</v>
       </c>
       <c r="E100" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>102</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C101" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" t="s">
+        <v>117</v>
+      </c>
+      <c r="E101" s="14">
         <v>45785</v>
       </c>
-      <c r="F100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" ht="27" customHeight="1" spans="2:2">
-      <c r="B102" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104">
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" ht="27" customHeight="1" spans="2:2">
+      <c r="B103" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
         <v>235</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="B105" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" t="s">
         <v>24</v>
       </c>
-      <c r="D104" t="s">
-        <v>118</v>
-      </c>
-      <c r="E104" s="14">
+      <c r="D105" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="14">
         <v>45786</v>
       </c>
-      <c r="F104" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" ht="24" customHeight="1" spans="2:2">
-      <c r="B106" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108">
-        <v>133</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C108" t="s">
-        <v>24</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="F105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" ht="24" customHeight="1" spans="2:2">
+      <c r="B107" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="E108" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F108" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>122</v>
@@ -2986,7 +2989,7 @@
         <v>123</v>
       </c>
       <c r="E109" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F109" t="s">
         <v>10</v>
@@ -2994,7 +2997,7 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>124</v>
@@ -3006,7 +3009,7 @@
         <v>125</v>
       </c>
       <c r="E110" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -3014,19 +3017,19 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>126</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D111" t="s">
         <v>127</v>
       </c>
       <c r="E111" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F111" t="s">
         <v>10</v>
@@ -3034,52 +3037,52 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>994</v>
+        <v>733</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>128</v>
       </c>
       <c r="C112" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D112" t="s">
         <v>129</v>
       </c>
       <c r="E112" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>994</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C113" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" t="s">
+        <v>131</v>
+      </c>
+      <c r="E113" s="14">
         <v>45834</v>
       </c>
-      <c r="F112" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" ht="29" customHeight="1" spans="2:2">
-      <c r="B114" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116">
-        <v>106</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C116" t="s">
-        <v>24</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" ht="29" customHeight="1" spans="2:2">
+      <c r="B115" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E116" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F116" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>133</v>
@@ -3091,76 +3094,96 @@
         <v>134</v>
       </c>
       <c r="E117" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
+        <v>207</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" t="s">
+        <v>24</v>
+      </c>
+      <c r="D118" t="s">
+        <v>136</v>
+      </c>
+      <c r="E118" s="14">
         <v>45817</v>
       </c>
-      <c r="F117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" ht="35" customHeight="1" spans="2:2">
-      <c r="B119" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121">
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" ht="35" customHeight="1" spans="2:2">
+      <c r="B120" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
         <v>127</v>
       </c>
-      <c r="B121" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C121" t="s">
-        <v>137</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="B122" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E121" s="14">
+      <c r="C122" t="s">
+        <v>139</v>
+      </c>
+      <c r="D122" t="s">
+        <v>140</v>
+      </c>
+      <c r="E122" s="14">
         <v>45831</v>
       </c>
-      <c r="F121" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" ht="41" customHeight="1" spans="1:2">
-      <c r="A127" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B127" s="19">
+      <c r="F122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" ht="41" customHeight="1" spans="1:2">
+      <c r="A128" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B128" s="18">
         <f>COUNT(A:A)</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="129" ht="30" customHeight="1" spans="1:2">
-      <c r="A129" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B129" s="21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="130" ht="30" customHeight="1" spans="1:2">
+      <c r="A130" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="130" ht="40" customHeight="1" spans="1:2">
-      <c r="A130" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B130" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="131" ht="40" customHeight="1" spans="1:2">
+      <c r="A131" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B131" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
         <v>31</v>
       </c>
     </row>
-    <row r="131" ht="36" customHeight="1" spans="1:2">
-      <c r="A131" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B131" s="25">
+    <row r="132" ht="36" customHeight="1" spans="1:2">
+      <c r="A132" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B132" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B121" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B122" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
3439. Reschedule Meetings for Maximum Free Time I (freegaps-array and Sliding Window)
</commit_message>
<xml_diff>
--- a/50  days challenge/Challenge_1_50days_tracker.xlsx
+++ b/50  days challenge/Challenge_1_50days_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="146">
   <si>
     <t>Q No.</t>
   </si>
@@ -158,7 +158,7 @@
     <t>Partition Array Such That Maximum Difference Is K</t>
   </si>
   <si>
-    <t xml:space="preserve">Arrays , Two pointer ,Sorting </t>
+    <t>Arrays , Two pointer ,Sorting</t>
   </si>
   <si>
     <t>Two pointers (Advance)</t>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Arrays ,Sliding Window ,Count</t>
+  </si>
+  <si>
+    <t>Reschedule Meetings for Maximum Free Time I</t>
   </si>
   <si>
     <t>Heap (Basics)</t>
@@ -1825,10 +1828,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -2463,418 +2466,418 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" ht="31" customHeight="1" spans="2:2">
-      <c r="B49" s="11" t="s">
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>3439</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>3066</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="14">
+        <v>45847</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" ht="31" customHeight="1" spans="2:2">
+      <c r="B50" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="C51" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" s="14">
-        <v>45701</v>
-      </c>
-      <c r="F51" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
+        <v>3066</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="14">
+        <v>45701</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>2099</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B53" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
         <v>8</v>
       </c>
-      <c r="D52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="14">
+      <c r="D53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" s="14">
         <v>45836</v>
       </c>
-      <c r="F52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" ht="38" customHeight="1" spans="2:2">
-      <c r="B54" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56">
-        <v>20</v>
-      </c>
-      <c r="B56" s="5" t="s">
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" ht="38" customHeight="1" spans="2:2">
+      <c r="B55" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C56" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" t="s">
-        <v>74</v>
-      </c>
-      <c r="E56" s="14">
-        <v>45719</v>
-      </c>
-      <c r="F56" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
+        <v>20</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" s="14">
+        <v>45719</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
         <v>155</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B58" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s">
         <v>24</v>
       </c>
-      <c r="D57" t="s">
-        <v>76</v>
-      </c>
-      <c r="E57" s="14">
+      <c r="D58" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="14">
         <v>45731</v>
       </c>
-      <c r="F57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" ht="40" customHeight="1" spans="2:2">
-      <c r="B59" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61">
+      <c r="F58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" ht="40" customHeight="1" spans="2:2">
+      <c r="B60" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
         <v>739</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B62" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
         <v>24</v>
       </c>
-      <c r="D61" t="s">
-        <v>79</v>
-      </c>
-      <c r="E61" s="14">
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="14">
         <v>45732</v>
       </c>
-      <c r="F61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" s="1" customFormat="1" spans="1:6">
-      <c r="A62" s="12">
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" s="1" customFormat="1" spans="1:6">
+      <c r="A63" s="12">
         <v>84</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B63" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E62" s="15">
+      <c r="E63" s="15">
         <v>45745</v>
       </c>
-      <c r="F62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" ht="34" customHeight="1" spans="2:2">
-      <c r="B64" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" ht="18" spans="1:6">
-      <c r="A66">
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" ht="34" customHeight="1" spans="2:2">
+      <c r="B65" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" ht="18" spans="1:6">
+      <c r="A67">
         <v>225</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B67" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" t="s">
         <v>8</v>
       </c>
-      <c r="D66" t="s">
-        <v>84</v>
-      </c>
-      <c r="E66" s="14">
+      <c r="D67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E67" s="14">
         <v>45841</v>
       </c>
-      <c r="F66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" customFormat="1" ht="31" customHeight="1" spans="2:2">
-      <c r="B68" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" customFormat="1" ht="18" spans="1:6">
-      <c r="A70">
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" customFormat="1" ht="31" customHeight="1" spans="2:2">
+      <c r="B69" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" customFormat="1" ht="18" spans="1:6">
+      <c r="A71">
         <v>206</v>
       </c>
-      <c r="B70" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="B71" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="E70" s="14">
-        <v>45746</v>
-      </c>
-      <c r="F70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" customFormat="1" spans="1:6">
-      <c r="A71">
-        <v>21</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
       </c>
       <c r="D71" t="s">
+        <v>88</v>
+      </c>
+      <c r="E71" s="14">
+        <v>45746</v>
+      </c>
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="1" spans="1:6">
+      <c r="A72">
+        <v>21</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E71" s="14">
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>90</v>
+      </c>
+      <c r="E72" s="14">
         <v>45747</v>
       </c>
-      <c r="F71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" customFormat="1" spans="5:5">
-      <c r="E72" s="14"/>
-    </row>
-    <row r="73" customFormat="1" ht="26" customHeight="1" spans="2:5">
-      <c r="B73" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" spans="5:5">
       <c r="E73" s="14"/>
     </row>
-    <row r="74" customFormat="1" spans="5:5">
+    <row r="74" customFormat="1" ht="26" customHeight="1" spans="2:5">
+      <c r="B74" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="E74" s="14"/>
     </row>
-    <row r="75" customFormat="1" spans="1:6">
-      <c r="A75">
-        <v>2</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" t="s">
-        <v>89</v>
-      </c>
-      <c r="E75" s="14">
-        <v>45747</v>
-      </c>
-      <c r="F75" t="s">
-        <v>10</v>
-      </c>
+    <row r="75" customFormat="1" spans="5:5">
+      <c r="E75" s="14"/>
     </row>
     <row r="76" customFormat="1" spans="1:6">
       <c r="A76">
-        <v>141</v>
+        <v>2</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C76" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" s="14">
+        <v>45747</v>
+      </c>
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="1" spans="1:6">
+      <c r="A77">
+        <v>141</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" t="s">
         <v>8</v>
       </c>
-      <c r="D76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E76" s="14">
+      <c r="D77" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" s="14">
         <v>45748</v>
       </c>
-      <c r="F76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" ht="35" customHeight="1" spans="2:2">
-      <c r="B78" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80">
-        <v>226</v>
-      </c>
-      <c r="B80" s="5" t="s">
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" ht="35" customHeight="1" spans="2:2">
+      <c r="B79" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="C80" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" t="s">
-        <v>96</v>
-      </c>
-      <c r="E80" s="14">
-        <v>45733</v>
-      </c>
-      <c r="F80" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>101</v>
+        <v>226</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
       </c>
       <c r="D81" t="s">
+        <v>97</v>
+      </c>
+      <c r="E81" s="14">
+        <v>45733</v>
+      </c>
+      <c r="F81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>101</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="14">
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>99</v>
+      </c>
+      <c r="E82" s="14">
         <v>45839</v>
       </c>
-      <c r="F81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" ht="39" customHeight="1" spans="2:2">
-      <c r="B83" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85">
-        <v>704</v>
-      </c>
-      <c r="B85" s="5" t="s">
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" ht="39" customHeight="1" spans="2:2">
+      <c r="B84" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="C85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" t="s">
-        <v>101</v>
-      </c>
-      <c r="E85" s="14">
-        <v>45757</v>
-      </c>
-      <c r="F85" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
+        <v>704</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86" s="14">
+        <v>45757</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
         <v>33</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B87" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" t="s">
         <v>24</v>
       </c>
-      <c r="D86" t="s">
-        <v>103</v>
-      </c>
-      <c r="E86" s="14">
+      <c r="D87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="14">
         <v>45759</v>
       </c>
-      <c r="F86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" ht="32" customHeight="1" spans="2:2">
-      <c r="B88" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="90" ht="30" customHeight="1" spans="1:6">
-      <c r="A90">
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" ht="32" customHeight="1" spans="2:2">
+      <c r="B89" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" ht="30" customHeight="1" spans="1:6">
+      <c r="A91">
         <v>34</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B91" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" t="s">
         <v>24</v>
       </c>
-      <c r="D90" t="s">
-        <v>106</v>
-      </c>
-      <c r="E90" s="14">
+      <c r="D91" t="s">
+        <v>107</v>
+      </c>
+      <c r="E91" s="14">
         <v>45773</v>
       </c>
-      <c r="F90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" ht="29" customHeight="1" spans="2:2">
-      <c r="B92" s="11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94">
-        <v>226</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="F91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" ht="29" customHeight="1" spans="2:2">
+      <c r="B93" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E94" s="14">
-        <v>45774</v>
-      </c>
-      <c r="F94" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
       </c>
       <c r="D95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E95" s="14">
-        <v>45782</v>
+        <v>45774</v>
       </c>
       <c r="F95" t="s">
         <v>10</v>
@@ -2882,134 +2885,134 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C96" t="s">
         <v>8</v>
       </c>
       <c r="D96" t="s">
+        <v>111</v>
+      </c>
+      <c r="E96" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
         <v>112</v>
       </c>
-      <c r="E96" s="14">
+      <c r="B97" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" t="s">
+        <v>113</v>
+      </c>
+      <c r="E97" s="14">
         <v>45842</v>
       </c>
-      <c r="F96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2">
-      <c r="B98" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100">
-        <v>100</v>
-      </c>
-      <c r="B100" s="5" t="s">
+      <c r="F97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100" t="s">
-        <v>115</v>
-      </c>
-      <c r="E100" s="14">
-        <v>45784</v>
-      </c>
-      <c r="F100" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>116</v>
+      </c>
+      <c r="E101" s="14">
+        <v>45784</v>
+      </c>
+      <c r="F101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
         <v>102</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B102" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102" t="s">
         <v>24</v>
       </c>
-      <c r="D101" t="s">
-        <v>117</v>
-      </c>
-      <c r="E101" s="14">
+      <c r="D102" t="s">
+        <v>118</v>
+      </c>
+      <c r="E102" s="14">
         <v>45785</v>
       </c>
-      <c r="F101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" ht="27" customHeight="1" spans="2:2">
-      <c r="B103" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105">
+      <c r="F102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" ht="27" customHeight="1" spans="2:2">
+      <c r="B104" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
         <v>235</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="B106" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C106" t="s">
         <v>24</v>
       </c>
-      <c r="D105" t="s">
-        <v>120</v>
-      </c>
-      <c r="E105" s="14">
+      <c r="D106" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="14">
         <v>45786</v>
       </c>
-      <c r="F105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" ht="24" customHeight="1" spans="2:2">
-      <c r="B107" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109">
-        <v>133</v>
-      </c>
-      <c r="B109" s="5" t="s">
+      <c r="F106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" ht="24" customHeight="1" spans="2:2">
+      <c r="B108" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="C109" t="s">
-        <v>24</v>
-      </c>
-      <c r="D109" t="s">
-        <v>123</v>
-      </c>
-      <c r="E109" s="14">
-        <v>45791</v>
-      </c>
-      <c r="F109" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>200</v>
+        <v>133</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C110" t="s">
         <v>24</v>
       </c>
       <c r="D110" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E110" s="14">
-        <v>45806</v>
+        <v>45791</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -3017,19 +3020,19 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>2359</v>
+        <v>200</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C111" t="s">
         <v>24</v>
       </c>
       <c r="D111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E111" s="14">
-        <v>45807</v>
+        <v>45806</v>
       </c>
       <c r="F111" t="s">
         <v>10</v>
@@ -3037,19 +3040,19 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>733</v>
+        <v>2359</v>
       </c>
       <c r="B112" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
         <v>128</v>
       </c>
-      <c r="C112" t="s">
-        <v>8</v>
-      </c>
-      <c r="D112" t="s">
-        <v>129</v>
-      </c>
       <c r="E112" s="14">
-        <v>45833</v>
+        <v>45807</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -3057,133 +3060,153 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
+        <v>733</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>130</v>
+      </c>
+      <c r="E113" s="14">
+        <v>45833</v>
+      </c>
+      <c r="F113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
         <v>994</v>
       </c>
-      <c r="B113" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="B114" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C114" t="s">
         <v>24</v>
       </c>
-      <c r="D113" t="s">
-        <v>131</v>
-      </c>
-      <c r="E113" s="14">
+      <c r="D114" t="s">
+        <v>132</v>
+      </c>
+      <c r="E114" s="14">
         <v>45834</v>
       </c>
-      <c r="F113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" ht="29" customHeight="1" spans="2:2">
-      <c r="B115" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117">
-        <v>106</v>
-      </c>
-      <c r="B117" s="5" t="s">
+      <c r="F114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" ht="29" customHeight="1" spans="2:2">
+      <c r="B116" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C117" t="s">
-        <v>24</v>
-      </c>
-      <c r="D117" t="s">
-        <v>134</v>
-      </c>
-      <c r="E117" s="14">
-        <v>45782</v>
-      </c>
-      <c r="F117" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>207</v>
+        <v>106</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C118" t="s">
         <v>24</v>
       </c>
       <c r="D118" t="s">
+        <v>135</v>
+      </c>
+      <c r="E118" s="14">
+        <v>45782</v>
+      </c>
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119">
+        <v>207</v>
+      </c>
+      <c r="B119" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E118" s="14">
+      <c r="C119" t="s">
+        <v>24</v>
+      </c>
+      <c r="D119" t="s">
+        <v>137</v>
+      </c>
+      <c r="E119" s="14">
         <v>45817</v>
       </c>
-      <c r="F118" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" ht="35" customHeight="1" spans="2:2">
-      <c r="B120" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122">
+      <c r="F119" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" ht="35" customHeight="1" spans="2:2">
+      <c r="B121" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
         <v>127</v>
       </c>
-      <c r="B122" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="C122" t="s">
+      <c r="B123" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D122" t="s">
+      <c r="C123" t="s">
         <v>140</v>
       </c>
-      <c r="E122" s="14">
+      <c r="D123" t="s">
+        <v>141</v>
+      </c>
+      <c r="E123" s="14">
         <v>45831</v>
       </c>
-      <c r="F122" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="128" ht="41" customHeight="1" spans="1:2">
-      <c r="A128" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B128" s="18">
+      <c r="F123" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" ht="41" customHeight="1" spans="1:2">
+      <c r="A129" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B129" s="18">
         <f>COUNT(A:A)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="130" ht="30" customHeight="1" spans="1:2">
-      <c r="A130" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="B130" s="20">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="131" ht="30" customHeight="1" spans="1:2">
+      <c r="A131" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B131" s="20">
         <f>COUNTIF(C:C,"Easy")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="131" ht="40" customHeight="1" spans="1:2">
-      <c r="A131" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B131" s="22">
+    <row r="132" ht="40" customHeight="1" spans="1:2">
+      <c r="A132" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B132" s="22">
         <f>COUNTIF(C:C,"Medium")</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="132" ht="36" customHeight="1" spans="1:2">
-      <c r="A132" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B132" s="24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="133" ht="36" customHeight="1" spans="1:2">
+      <c r="A133" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B133" s="24">
         <f>COUNTIF(C:C,"Hard")</f>
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B122" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
+    <hyperlink ref="B123" r:id="rId1" display="127. Word Ladder" tooltip="https://leetcode.com/problems/word-ladder/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>